<commit_message>
more sensible modes analysis
incorporating PA and Mode into phonetic parameter analysis!
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/output/Ch_7_Mode_PA_Params_Tables_Graphs.xlsx
+++ b/Ch_7_Sentence_Modes/output/Ch_7_Mode_PA_Params_Tables_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A3F454-F260-4201-AA46-8544C90E4700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF4D75A-3319-44AE-879A-1364D4CA951E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11060" yWindow="-18020" windowWidth="17340" windowHeight="9250" activeTab="3" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="3" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Intercepts" sheetId="1" r:id="rId1"/>
@@ -1554,6 +1554,18 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="12" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1590,28 +1602,16 @@
     <xf numFmtId="2" fontId="12" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="12" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5812,16 +5812,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>11.165000000000006</c:v>
+                    <c:v>10.796000000000006</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.824999999999996</c:v>
+                    <c:v>24.936</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.854999999999997</c:v>
+                    <c:v>16.801000000000009</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>11.678000000000004</c:v>
+                    <c:v>16.794999999999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -5833,16 +5833,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>11.165000000000006</c:v>
+                    <c:v>10.796000000000006</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.824999999999996</c:v>
+                    <c:v>24.936</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.854999999999997</c:v>
+                    <c:v>16.801000000000009</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>11.678000000000004</c:v>
+                    <c:v>16.794999999999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -5882,16 +5882,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>93.504000000000005</c:v>
+                  <c:v>96.254000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.188999999999993</c:v>
+                  <c:v>87.087000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.698999999999998</c:v>
+                  <c:v>73.647000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.016000000000005</c:v>
+                  <c:v>69.733999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6465,16 +6465,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.4920000000000044</c:v>
+                    <c:v>2.3449999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7489999999999952</c:v>
+                    <c:v>2.9230000000000018</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5319999999999965</c:v>
+                    <c:v>2.4909999999999997</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.5039999999999907</c:v>
+                    <c:v>2.7789999999999964</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -6486,16 +6486,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.4920000000000044</c:v>
+                    <c:v>2.3449999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7489999999999952</c:v>
+                    <c:v>2.9230000000000018</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5319999999999965</c:v>
+                    <c:v>2.4909999999999997</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.5039999999999907</c:v>
+                    <c:v>2.7789999999999964</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -6531,16 +6531,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>87.239000000000004</c:v>
+                  <c:v>86.994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.323999999999998</c:v>
+                  <c:v>91.176000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.745999999999995</c:v>
+                  <c:v>88.528999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.081999999999994</c:v>
+                  <c:v>90.988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6666,16 +6666,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.6670000000000016</c:v>
+                    <c:v>2.5400000000000063</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.1290000000000049</c:v>
+                    <c:v>3.4869999999999948</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7409999999999997</c:v>
+                    <c:v>2.9799999999999898</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.6880000000000024</c:v>
+                    <c:v>3.0679999999999978</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -6687,16 +6687,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.6670000000000016</c:v>
+                    <c:v>2.5400000000000063</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.1290000000000049</c:v>
+                    <c:v>3.4869999999999948</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.7409999999999997</c:v>
+                    <c:v>2.9799999999999898</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.6880000000000024</c:v>
+                    <c:v>3.0679999999999978</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -6739,16 +6739,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>93.153000000000006</c:v>
+                  <c:v>92.605000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.519000000000005</c:v>
+                  <c:v>93.893000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.807000000000002</c:v>
+                  <c:v>98.281999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.397999999999996</c:v>
+                  <c:v>98.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8098,7 +8098,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>11.165000000000006</c:v>
+                    <c:v>10.796000000000006</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>50.658999999999992</c:v>
@@ -8113,7 +8113,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>11.165000000000006</c:v>
+                    <c:v>10.796000000000006</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>50.658999999999992</c:v>
@@ -8141,10 +8141,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.4920000000000044</c:v>
+                    <c:v>2.3449999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6670000000000016</c:v>
+                    <c:v>2.5400000000000063</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8156,10 +8156,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.4920000000000044</c:v>
+                    <c:v>2.3449999999999989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6670000000000016</c:v>
+                    <c:v>2.5400000000000063</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8179,7 +8179,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>93.504000000000005</c:v>
+                  <c:v>96.254000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>316.149</c:v>
@@ -8194,10 +8194,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>87.239000000000004</c:v>
+                  <c:v>86.994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.153000000000006</c:v>
+                  <c:v>92.605000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8256,7 +8256,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>19.824999999999996</c:v>
+                    <c:v>24.936</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>56.068999999999988</c:v>
@@ -8271,7 +8271,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>19.824999999999996</c:v>
+                    <c:v>24.936</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>56.068999999999988</c:v>
@@ -8299,10 +8299,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.7489999999999952</c:v>
+                    <c:v>2.9230000000000018</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.1290000000000049</c:v>
+                    <c:v>3.4869999999999948</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8314,10 +8314,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.7489999999999952</c:v>
+                    <c:v>2.9230000000000018</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.1290000000000049</c:v>
+                    <c:v>3.4869999999999948</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8337,7 +8337,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>82.188999999999993</c:v>
+                  <c:v>87.087000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>237.262</c:v>
@@ -8352,10 +8352,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>91.323999999999998</c:v>
+                  <c:v>91.176000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.519000000000005</c:v>
+                  <c:v>93.893000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8414,7 +8414,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>12.854999999999997</c:v>
+                    <c:v>16.801000000000009</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>51.513000000000005</c:v>
@@ -8429,7 +8429,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>12.854999999999997</c:v>
+                    <c:v>16.801000000000009</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>51.513000000000005</c:v>
@@ -8457,10 +8457,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.5319999999999965</c:v>
+                    <c:v>2.4909999999999997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7409999999999997</c:v>
+                    <c:v>2.9799999999999898</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8472,10 +8472,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.5319999999999965</c:v>
+                    <c:v>2.4909999999999997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7409999999999997</c:v>
+                    <c:v>2.9799999999999898</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8495,7 +8495,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>72.698999999999998</c:v>
+                  <c:v>73.647000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>300.93700000000001</c:v>
@@ -8510,10 +8510,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>88.745999999999995</c:v>
+                  <c:v>88.528999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.807000000000002</c:v>
+                  <c:v>98.281999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8575,7 +8575,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>11.678000000000004</c:v>
+                    <c:v>16.794999999999995</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>50.907999999999987</c:v>
@@ -8590,7 +8590,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>11.678000000000004</c:v>
+                    <c:v>16.794999999999995</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>50.907999999999987</c:v>
@@ -8618,10 +8618,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.5039999999999907</c:v>
+                    <c:v>2.7789999999999964</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6880000000000024</c:v>
+                    <c:v>3.0679999999999978</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8633,10 +8633,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>2.5039999999999907</c:v>
+                    <c:v>2.7789999999999964</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.6880000000000024</c:v>
+                    <c:v>3.0679999999999978</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -8656,7 +8656,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>70.016000000000005</c:v>
+                  <c:v>69.733999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>298.25299999999999</c:v>
@@ -8671,10 +8671,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>91.081999999999994</c:v>
+                  <c:v>90.988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.397999999999996</c:v>
+                  <c:v>98.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10194,28 +10194,28 @@
             <v>L*H</v>
           </cell>
           <cell r="B2">
-            <v>93.504000000000005</v>
+            <v>96.254000000000005</v>
           </cell>
           <cell r="C2">
-            <v>5.6959999999999997</v>
+            <v>5.508</v>
           </cell>
           <cell r="D2">
-            <v>82.338999999999999</v>
+            <v>85.457999999999998</v>
           </cell>
           <cell r="E2">
-            <v>104.66800000000001</v>
+            <v>107.04900000000001</v>
           </cell>
           <cell r="F2">
-            <v>16.414999999999999</v>
+            <v>17.475000000000001</v>
           </cell>
           <cell r="G2">
-            <v>9.94</v>
+            <v>11.23</v>
           </cell>
           <cell r="H2">
-            <v>1.5799999999999999E-8</v>
+            <v>1.7100000000000001E-9</v>
           </cell>
           <cell r="I2">
-            <v>1.11E-7</v>
+            <v>1.37E-8</v>
           </cell>
         </row>
         <row r="3">
@@ -10223,28 +10223,28 @@
             <v>^[L*]H</v>
           </cell>
           <cell r="B3">
-            <v>82.188999999999993</v>
+            <v>87.087000000000003</v>
           </cell>
           <cell r="C3">
-            <v>10.115</v>
+            <v>12.723000000000001</v>
           </cell>
           <cell r="D3">
-            <v>62.363999999999997</v>
+            <v>62.151000000000003</v>
           </cell>
           <cell r="E3">
-            <v>102.014</v>
+            <v>112.023</v>
           </cell>
           <cell r="F3">
-            <v>8.1259999999999994</v>
+            <v>6.8449999999999998</v>
           </cell>
           <cell r="G3">
-            <v>90.27</v>
+            <v>0</v>
           </cell>
           <cell r="H3">
-            <v>2.2100000000000001E-12</v>
+            <v>1</v>
           </cell>
           <cell r="I3">
-            <v>1.54E-11</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="4">
@@ -10252,28 +10252,28 @@
             <v>L*^[H]</v>
           </cell>
           <cell r="B4">
-            <v>72.698999999999998</v>
+            <v>73.647000000000006</v>
           </cell>
           <cell r="C4">
-            <v>6.5590000000000002</v>
+            <v>8.5719999999999992</v>
           </cell>
           <cell r="D4">
-            <v>59.844000000000001</v>
+            <v>56.845999999999997</v>
           </cell>
           <cell r="E4">
-            <v>85.552999999999997</v>
+            <v>90.448999999999998</v>
           </cell>
           <cell r="F4">
-            <v>11.084</v>
+            <v>8.5909999999999993</v>
           </cell>
           <cell r="G4">
-            <v>17.399999999999999</v>
+            <v>8.49</v>
           </cell>
           <cell r="H4">
-            <v>2.6000000000000001E-9</v>
+            <v>1.8099999999999999E-5</v>
           </cell>
           <cell r="I4">
-            <v>1.8200000000000001E-8</v>
+            <v>1.45E-4</v>
           </cell>
         </row>
         <row r="5">
@@ -10281,28 +10281,28 @@
             <v>^[L*H]</v>
           </cell>
           <cell r="B5">
-            <v>70.016000000000005</v>
+            <v>69.733999999999995</v>
           </cell>
           <cell r="C5">
-            <v>5.9580000000000002</v>
+            <v>8.5690000000000008</v>
           </cell>
           <cell r="D5">
-            <v>58.338000000000001</v>
+            <v>52.939</v>
           </cell>
           <cell r="E5">
-            <v>81.694000000000003</v>
+            <v>86.528000000000006</v>
           </cell>
           <cell r="F5">
-            <v>11.750999999999999</v>
+            <v>8.1379999999999999</v>
           </cell>
           <cell r="G5">
-            <v>11.89</v>
+            <v>10.3</v>
           </cell>
           <cell r="H5">
-            <v>6.6899999999999997E-8</v>
+            <v>8.4400000000000005E-6</v>
           </cell>
           <cell r="I5">
-            <v>4.6899999999999998E-7</v>
+            <v>6.7500000000000001E-5</v>
           </cell>
         </row>
       </sheetData>
@@ -10321,12 +10321,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.73093594252433203</v>
+            <v>0.80115699175044897</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.593435532261537</v>
+            <v>0.62408082900844397</v>
           </cell>
         </row>
       </sheetData>
@@ -10596,126 +10596,126 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="C2">
-            <v>4.085</v>
+            <v>4.3390000000000004</v>
           </cell>
           <cell r="D2">
-            <v>0.58599999999999997</v>
+            <v>1.3</v>
           </cell>
           <cell r="E2">
-            <v>2.9359999999999999</v>
+            <v>1.79</v>
           </cell>
           <cell r="F2">
-            <v>5.2350000000000003</v>
+            <v>6.8879999999999999</v>
           </cell>
           <cell r="G2">
-            <v>6.9660000000000002</v>
+            <v>3.3370000000000002</v>
           </cell>
           <cell r="H2">
-            <v>613.48</v>
+            <v>1.94</v>
           </cell>
           <cell r="I2">
-            <v>8.4099999999999999E-12</v>
+            <v>8.2500000000000004E-2</v>
           </cell>
           <cell r="J2">
-            <v>5.8899999999999998E-11</v>
+            <v>0.6603</v>
           </cell>
         </row>
         <row r="3">
           <cell r="C3">
-            <v>1.5069999999999999</v>
+            <v>1.536</v>
           </cell>
           <cell r="D3">
-            <v>0.251</v>
+            <v>0.41899999999999998</v>
           </cell>
           <cell r="E3">
-            <v>1.0149999999999999</v>
+            <v>0.71499999999999997</v>
           </cell>
           <cell r="F3">
-            <v>2</v>
+            <v>2.3559999999999999</v>
           </cell>
           <cell r="G3">
-            <v>6.0039999999999996</v>
+            <v>3.6680000000000001</v>
           </cell>
           <cell r="H3">
-            <v>613.33000000000004</v>
+            <v>1.73</v>
           </cell>
           <cell r="I3">
-            <v>3.3000000000000002E-9</v>
+            <v>8.2600000000000007E-2</v>
           </cell>
         </row>
         <row r="4">
           <cell r="C4">
-            <v>3.843</v>
+            <v>3.9940000000000002</v>
           </cell>
           <cell r="D4">
-            <v>0.14099999999999999</v>
+            <v>0.61499999999999999</v>
           </cell>
           <cell r="E4">
-            <v>3.5659999999999998</v>
+            <v>2.7890000000000001</v>
           </cell>
           <cell r="F4">
-            <v>4.12</v>
+            <v>5.1989999999999998</v>
           </cell>
           <cell r="G4">
-            <v>27.239000000000001</v>
+            <v>6.4980000000000002</v>
           </cell>
           <cell r="H4">
-            <v>613.19000000000005</v>
+            <v>8.8800000000000008</v>
           </cell>
           <cell r="I4">
-            <v>1.12E-107</v>
+            <v>1.1900000000000001E-4</v>
           </cell>
           <cell r="J4">
-            <v>7.8599999999999994E-107</v>
+            <v>9.5E-4</v>
           </cell>
         </row>
         <row r="5">
           <cell r="C5">
-            <v>-2.5779999999999998</v>
+            <v>-2.6469999999999998</v>
           </cell>
           <cell r="D5">
-            <v>0.63900000000000001</v>
+            <v>0.96</v>
           </cell>
           <cell r="E5">
-            <v>-3.8290000000000002</v>
+            <v>-4.5279999999999996</v>
           </cell>
           <cell r="F5">
-            <v>-1.3260000000000001</v>
+            <v>-0.76500000000000001</v>
           </cell>
           <cell r="G5">
-            <v>-4.0369999999999999</v>
+            <v>-2.7570000000000001</v>
           </cell>
           <cell r="H5">
-            <v>613.48</v>
+            <v>0</v>
           </cell>
           <cell r="I5">
-            <v>6.0999999999999999E-5</v>
+            <v>0.99990000000000001</v>
           </cell>
           <cell r="J5">
-            <v>4.2700000000000002E-4</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6">
-            <v>-0.24199999999999999</v>
+            <v>-0.188</v>
           </cell>
           <cell r="D6">
-            <v>0.58799999999999997</v>
+            <v>1.0129999999999999</v>
           </cell>
           <cell r="E6">
-            <v>-1.3939999999999999</v>
+            <v>-2.1739999999999999</v>
           </cell>
           <cell r="F6">
-            <v>0.90900000000000003</v>
+            <v>1.798</v>
           </cell>
           <cell r="G6">
-            <v>-0.41199999999999998</v>
+            <v>-0.186</v>
           </cell>
           <cell r="H6">
-            <v>613.44000000000005</v>
+            <v>0</v>
           </cell>
           <cell r="I6">
-            <v>0.68030000000000002</v>
+            <v>0.99919999999999998</v>
           </cell>
           <cell r="J6">
             <v>0.99990000000000001</v>
@@ -10723,28 +10723,28 @@
         </row>
         <row r="7">
           <cell r="C7">
-            <v>2.3359999999999999</v>
+            <v>2.4590000000000001</v>
           </cell>
           <cell r="D7">
-            <v>0.27900000000000003</v>
+            <v>0.68200000000000005</v>
           </cell>
           <cell r="E7">
-            <v>1.79</v>
+            <v>1.1220000000000001</v>
           </cell>
           <cell r="F7">
-            <v>2.8820000000000001</v>
+            <v>3.7949999999999999</v>
           </cell>
           <cell r="G7">
-            <v>8.3840000000000003</v>
+            <v>3.6040000000000001</v>
           </cell>
           <cell r="H7">
-            <v>613.32000000000005</v>
+            <v>8.08</v>
           </cell>
           <cell r="I7">
-            <v>3.52E-16</v>
+            <v>6.7999999999999996E-3</v>
           </cell>
           <cell r="J7">
-            <v>2.4699999999999999E-15</v>
+            <v>5.4600000000000003E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -10763,152 +10763,152 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="C2">
-            <v>1.367</v>
+            <v>1.145</v>
           </cell>
           <cell r="D2">
-            <v>0.82699999999999996</v>
+            <v>1.8109999999999999</v>
           </cell>
           <cell r="E2">
-            <v>-0.255</v>
+            <v>-2.4049999999999998</v>
           </cell>
           <cell r="F2">
-            <v>2.988</v>
+            <v>4.6950000000000003</v>
           </cell>
           <cell r="G2">
-            <v>1.6519999999999999</v>
+            <v>0.63200000000000001</v>
           </cell>
           <cell r="H2">
-            <v>617.80999999999995</v>
+            <v>0</v>
           </cell>
           <cell r="I2">
-            <v>9.9000000000000005E-2</v>
+            <v>1</v>
           </cell>
           <cell r="J2">
-            <v>0.69310000000000005</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="3">
           <cell r="C3">
-            <v>5.6539999999999999</v>
+            <v>5.6769999999999996</v>
           </cell>
           <cell r="D3">
-            <v>0.35399999999999998</v>
+            <v>0.625</v>
           </cell>
           <cell r="E3">
-            <v>4.96</v>
+            <v>4.452</v>
           </cell>
           <cell r="F3">
-            <v>6.3490000000000002</v>
+            <v>6.9020000000000001</v>
           </cell>
           <cell r="G3">
-            <v>15.965</v>
+            <v>9.0860000000000003</v>
           </cell>
           <cell r="H3">
-            <v>617.54</v>
+            <v>2.83</v>
           </cell>
           <cell r="I3">
-            <v>2.7500000000000002E-48</v>
+            <v>3.5000000000000001E-3</v>
           </cell>
         </row>
         <row r="4">
           <cell r="C4">
-            <v>5.2460000000000004</v>
+            <v>5.5650000000000004</v>
           </cell>
           <cell r="D4">
-            <v>0.19700000000000001</v>
+            <v>0.72499999999999998</v>
           </cell>
           <cell r="E4">
-            <v>4.8600000000000003</v>
+            <v>4.1449999999999996</v>
           </cell>
           <cell r="F4">
-            <v>5.6319999999999997</v>
+            <v>6.9850000000000003</v>
           </cell>
           <cell r="G4">
-            <v>26.620999999999999</v>
+            <v>7.6820000000000004</v>
           </cell>
           <cell r="H4">
-            <v>617.32000000000005</v>
+            <v>9.24</v>
           </cell>
           <cell r="I4">
-            <v>1.43E-104</v>
+            <v>2.6299999999999999E-5</v>
           </cell>
           <cell r="J4">
-            <v>9.9999999999999996E-104</v>
+            <v>2.1100000000000001E-4</v>
           </cell>
         </row>
         <row r="5">
           <cell r="C5">
-            <v>4.2880000000000003</v>
+            <v>4.3890000000000002</v>
           </cell>
           <cell r="D5">
-            <v>0.9</v>
+            <v>1.331</v>
           </cell>
           <cell r="E5">
-            <v>2.5230000000000001</v>
+            <v>1.7809999999999999</v>
           </cell>
           <cell r="F5">
-            <v>6.0519999999999996</v>
+            <v>6.9969999999999999</v>
           </cell>
           <cell r="G5">
-            <v>4.7629999999999999</v>
+            <v>3.2989999999999999</v>
           </cell>
           <cell r="H5">
-            <v>617.79999999999995</v>
+            <v>0</v>
           </cell>
           <cell r="I5">
-            <v>2.3800000000000001E-6</v>
+            <v>0.99870000000000003</v>
           </cell>
           <cell r="J5">
-            <v>1.66E-5</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6">
-            <v>3.879</v>
+            <v>4.2770000000000001</v>
           </cell>
           <cell r="D6">
-            <v>0.82899999999999996</v>
+            <v>1.31</v>
           </cell>
           <cell r="E6">
-            <v>2.254</v>
+            <v>1.71</v>
           </cell>
           <cell r="F6">
-            <v>5.5049999999999999</v>
+            <v>6.8449999999999998</v>
           </cell>
           <cell r="G6">
-            <v>4.6769999999999996</v>
+            <v>3.266</v>
           </cell>
           <cell r="H6">
-            <v>617.75</v>
+            <v>0</v>
           </cell>
           <cell r="I6">
-            <v>3.58E-6</v>
+            <v>0.99880000000000002</v>
           </cell>
           <cell r="J6">
-            <v>2.5000000000000001E-5</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>-0.40899999999999997</v>
+            <v>-0.112</v>
           </cell>
           <cell r="D7">
-            <v>0.39100000000000001</v>
+            <v>0.82099999999999995</v>
           </cell>
           <cell r="E7">
-            <v>-1.1739999999999999</v>
+            <v>-1.722</v>
           </cell>
           <cell r="F7">
-            <v>0.35699999999999998</v>
+            <v>1.498</v>
           </cell>
           <cell r="G7">
-            <v>-1.046</v>
+            <v>-0.13600000000000001</v>
           </cell>
           <cell r="H7">
-            <v>617.5</v>
+            <v>6.82</v>
           </cell>
           <cell r="I7">
-            <v>0.29599999999999999</v>
+            <v>0.89570000000000005</v>
           </cell>
           <cell r="J7">
             <v>0.99990000000000001</v>
@@ -10930,25 +10930,25 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="C2">
-            <v>-11.315</v>
+            <v>-10.675000000000001</v>
           </cell>
           <cell r="D2">
-            <v>8.2789999999999999</v>
+            <v>18.943999999999999</v>
           </cell>
           <cell r="E2">
-            <v>-27.542000000000002</v>
+            <v>-47.805999999999997</v>
           </cell>
           <cell r="F2">
-            <v>4.9119999999999999</v>
+            <v>26.454999999999998</v>
           </cell>
           <cell r="G2">
-            <v>-1.367</v>
+            <v>-0.56399999999999995</v>
           </cell>
           <cell r="H2">
-            <v>619.9</v>
+            <v>0.05</v>
           </cell>
           <cell r="I2">
-            <v>0.17219999999999999</v>
+            <v>0.92359999999999998</v>
           </cell>
           <cell r="J2">
             <v>0.99990000000000001</v>
@@ -10956,74 +10956,74 @@
         </row>
         <row r="3">
           <cell r="C3">
-            <v>-20.805</v>
+            <v>-22.606000000000002</v>
           </cell>
           <cell r="D3">
-            <v>3.5419999999999998</v>
+            <v>4.3220000000000001</v>
           </cell>
           <cell r="E3">
-            <v>-27.748000000000001</v>
+            <v>-31.077000000000002</v>
           </cell>
           <cell r="F3">
-            <v>-13.862</v>
+            <v>-14.135999999999999</v>
           </cell>
           <cell r="G3">
-            <v>-5.8730000000000002</v>
+            <v>-5.2309999999999999</v>
           </cell>
           <cell r="H3">
-            <v>617.97</v>
+            <v>6.16</v>
           </cell>
           <cell r="I3">
-            <v>6.9900000000000001E-9</v>
+            <v>1.8E-3</v>
           </cell>
         </row>
         <row r="4">
           <cell r="C4">
-            <v>-23.488</v>
+            <v>-26.52</v>
           </cell>
           <cell r="D4">
-            <v>1.98</v>
+            <v>7.0949999999999998</v>
           </cell>
           <cell r="E4">
-            <v>-27.369</v>
+            <v>-40.426000000000002</v>
           </cell>
           <cell r="F4">
-            <v>-19.606999999999999</v>
+            <v>-12.614000000000001</v>
           </cell>
           <cell r="G4">
-            <v>-11.861000000000001</v>
+            <v>-3.738</v>
           </cell>
           <cell r="H4">
-            <v>617.84</v>
+            <v>8.81</v>
           </cell>
           <cell r="I4">
-            <v>2.2199999999999999E-29</v>
+            <v>4.7999999999999996E-3</v>
           </cell>
           <cell r="J4">
-            <v>1.55E-28</v>
+            <v>3.8600000000000002E-2</v>
           </cell>
         </row>
         <row r="5">
           <cell r="C5">
-            <v>-9.49</v>
+            <v>-13.439</v>
           </cell>
           <cell r="D5">
-            <v>8.9979999999999993</v>
+            <v>12.378</v>
           </cell>
           <cell r="E5">
-            <v>-27.126000000000001</v>
+            <v>-37.701000000000001</v>
           </cell>
           <cell r="F5">
-            <v>8.1449999999999996</v>
+            <v>10.821999999999999</v>
           </cell>
           <cell r="G5">
-            <v>-1.0549999999999999</v>
+            <v>-1.0860000000000001</v>
           </cell>
           <cell r="H5">
-            <v>619.15</v>
+            <v>0</v>
           </cell>
           <cell r="I5">
-            <v>0.29199999999999998</v>
+            <v>1</v>
           </cell>
           <cell r="J5">
             <v>0.99990000000000001</v>
@@ -11031,25 +11031,25 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>-12.173</v>
+            <v>-17.353000000000002</v>
           </cell>
           <cell r="D6">
-            <v>8.32</v>
+            <v>12.58</v>
           </cell>
           <cell r="E6">
-            <v>-28.48</v>
+            <v>-42.01</v>
           </cell>
           <cell r="F6">
-            <v>4.1340000000000003</v>
+            <v>7.3040000000000003</v>
           </cell>
           <cell r="G6">
-            <v>-1.4630000000000001</v>
+            <v>-1.379</v>
           </cell>
           <cell r="H6">
-            <v>619.98</v>
+            <v>0</v>
           </cell>
           <cell r="I6">
-            <v>0.1439</v>
+            <v>1</v>
           </cell>
           <cell r="J6">
             <v>0.99990000000000001</v>
@@ -11057,25 +11057,25 @@
         </row>
         <row r="7">
           <cell r="C7">
-            <v>-2.6829999999999998</v>
+            <v>-3.9129999999999998</v>
           </cell>
           <cell r="D7">
-            <v>3.9220000000000002</v>
+            <v>8.3190000000000008</v>
           </cell>
           <cell r="E7">
-            <v>-10.37</v>
+            <v>-20.219000000000001</v>
           </cell>
           <cell r="F7">
-            <v>5.0039999999999996</v>
+            <v>12.391999999999999</v>
           </cell>
           <cell r="G7">
-            <v>-0.68400000000000005</v>
+            <v>-0.47</v>
           </cell>
           <cell r="H7">
-            <v>618.83000000000004</v>
+            <v>10.050000000000001</v>
           </cell>
           <cell r="I7">
-            <v>0.49419999999999997</v>
+            <v>0.64810000000000001</v>
           </cell>
           <cell r="J7">
             <v>0.99990000000000001</v>
@@ -11118,7 +11118,7 @@
             <v>1.7000000000000001E-10</v>
           </cell>
           <cell r="J2">
-            <v>1.19E-9</v>
+            <v>1.3600000000000001E-9</v>
           </cell>
         </row>
         <row r="3">
@@ -11167,7 +11167,7 @@
             <v>1.27E-9</v>
           </cell>
           <cell r="J4">
-            <v>8.9199999999999998E-9</v>
+            <v>1.02E-8</v>
           </cell>
         </row>
         <row r="5">
@@ -11193,7 +11193,7 @@
             <v>1.75E-6</v>
           </cell>
           <cell r="J5">
-            <v>1.2300000000000001E-5</v>
+            <v>1.4E-5</v>
           </cell>
         </row>
         <row r="6">
@@ -11219,7 +11219,7 @@
             <v>7.6799999999999999E-7</v>
           </cell>
           <cell r="J6">
-            <v>5.3800000000000002E-6</v>
+            <v>6.1399999999999997E-6</v>
           </cell>
         </row>
         <row r="7">
@@ -11434,28 +11434,28 @@
             <v>L*H</v>
           </cell>
           <cell r="B2">
-            <v>87.239000000000004</v>
+            <v>86.994</v>
           </cell>
           <cell r="C2">
-            <v>1.2709999999999999</v>
+            <v>1.196</v>
           </cell>
           <cell r="D2">
-            <v>84.747</v>
+            <v>84.649000000000001</v>
           </cell>
           <cell r="E2">
-            <v>89.730999999999995</v>
+            <v>89.337999999999994</v>
           </cell>
           <cell r="F2">
-            <v>68.623000000000005</v>
+            <v>72.718999999999994</v>
           </cell>
           <cell r="G2">
-            <v>9.01</v>
+            <v>9.1999999999999993</v>
           </cell>
           <cell r="H2">
-            <v>1.4600000000000001E-13</v>
+            <v>5.1600000000000002E-14</v>
           </cell>
           <cell r="I2">
-            <v>1.0200000000000001E-12</v>
+            <v>4.1300000000000001E-13</v>
           </cell>
         </row>
         <row r="3">
@@ -11463,28 +11463,28 @@
             <v>^[L*]H</v>
           </cell>
           <cell r="B3">
-            <v>91.323999999999998</v>
+            <v>91.176000000000002</v>
           </cell>
           <cell r="C3">
-            <v>1.403</v>
+            <v>1.4910000000000001</v>
           </cell>
           <cell r="D3">
-            <v>88.575000000000003</v>
+            <v>88.253</v>
           </cell>
           <cell r="E3">
-            <v>94.072999999999993</v>
+            <v>94.099000000000004</v>
           </cell>
           <cell r="F3">
-            <v>65.114000000000004</v>
+            <v>61.14</v>
           </cell>
           <cell r="G3">
-            <v>13.34</v>
+            <v>0</v>
           </cell>
           <cell r="H3">
-            <v>4.34E-18</v>
+            <v>0.99970000000000003</v>
           </cell>
           <cell r="I3">
-            <v>3.0399999999999998E-17</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="4">
@@ -11492,19 +11492,19 @@
             <v>L*^[H]</v>
           </cell>
           <cell r="B4">
-            <v>88.745999999999995</v>
+            <v>88.528999999999996</v>
           </cell>
           <cell r="C4">
-            <v>1.292</v>
+            <v>1.2709999999999999</v>
           </cell>
           <cell r="D4">
-            <v>86.213999999999999</v>
+            <v>86.037999999999997</v>
           </cell>
           <cell r="E4">
-            <v>91.278999999999996</v>
+            <v>91.02</v>
           </cell>
           <cell r="I4">
-            <v>2.0399999999999999E-13</v>
+            <v>6.0099999999999996E-13</v>
           </cell>
         </row>
         <row r="5">
@@ -11512,19 +11512,19 @@
             <v>^[L*H]</v>
           </cell>
           <cell r="B5">
-            <v>91.081999999999994</v>
+            <v>90.988</v>
           </cell>
           <cell r="C5">
-            <v>1.2769999999999999</v>
+            <v>1.4179999999999999</v>
           </cell>
           <cell r="D5">
-            <v>88.578000000000003</v>
+            <v>88.209000000000003</v>
           </cell>
           <cell r="E5">
-            <v>93.585999999999999</v>
+            <v>93.766000000000005</v>
           </cell>
           <cell r="I5">
-            <v>4.4800000000000001E-13</v>
+            <v>1.8899999999999999E-15</v>
           </cell>
         </row>
       </sheetData>
@@ -11670,7 +11670,7 @@
             <v>1.5E-3</v>
           </cell>
           <cell r="I2">
-            <v>1.03E-2</v>
+            <v>1.18E-2</v>
           </cell>
         </row>
         <row r="3">
@@ -11699,7 +11699,7 @@
             <v>8.43E-4</v>
           </cell>
           <cell r="I3">
-            <v>5.8999999999999999E-3</v>
+            <v>6.7000000000000002E-3</v>
           </cell>
         </row>
         <row r="4">
@@ -11728,7 +11728,7 @@
             <v>1.2999999999999999E-3</v>
           </cell>
           <cell r="I4">
-            <v>9.1000000000000004E-3</v>
+            <v>1.04E-2</v>
           </cell>
         </row>
         <row r="5">
@@ -11757,7 +11757,7 @@
             <v>1.6000000000000001E-3</v>
           </cell>
           <cell r="I5">
-            <v>1.12E-2</v>
+            <v>1.2800000000000001E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -11779,28 +11779,28 @@
             <v>L*H</v>
           </cell>
           <cell r="B2">
-            <v>93.153000000000006</v>
+            <v>92.605000000000004</v>
           </cell>
           <cell r="C2">
-            <v>1.36</v>
+            <v>1.296</v>
           </cell>
           <cell r="D2">
-            <v>90.486000000000004</v>
+            <v>90.064999999999998</v>
           </cell>
           <cell r="E2">
-            <v>95.819000000000003</v>
+            <v>95.144000000000005</v>
           </cell>
           <cell r="F2">
-            <v>68.471999999999994</v>
+            <v>71.475999999999999</v>
           </cell>
           <cell r="G2">
-            <v>9.02</v>
+            <v>9.14</v>
           </cell>
           <cell r="H2">
-            <v>1.4499999999999999E-13</v>
+            <v>7.0700000000000004E-14</v>
           </cell>
           <cell r="I2">
-            <v>1.0200000000000001E-12</v>
+            <v>5.6500000000000002E-13</v>
           </cell>
         </row>
         <row r="3">
@@ -11808,28 +11808,28 @@
             <v>^[L*]H</v>
           </cell>
           <cell r="B3">
-            <v>94.519000000000005</v>
+            <v>93.893000000000001</v>
           </cell>
           <cell r="C3">
-            <v>1.5960000000000001</v>
+            <v>1.7789999999999999</v>
           </cell>
           <cell r="D3">
-            <v>91.39</v>
+            <v>90.406000000000006</v>
           </cell>
           <cell r="E3">
-            <v>97.647999999999996</v>
+            <v>97.379000000000005</v>
           </cell>
           <cell r="F3">
-            <v>59.206000000000003</v>
+            <v>52.786999999999999</v>
           </cell>
           <cell r="G3">
-            <v>17.059999999999999</v>
+            <v>0</v>
           </cell>
           <cell r="H3">
-            <v>3.4500000000000002E-21</v>
+            <v>0.99439999999999995</v>
           </cell>
           <cell r="I3">
-            <v>2.42E-20</v>
+            <v>0.99990000000000001</v>
           </cell>
         </row>
         <row r="4">
@@ -11837,19 +11837,19 @@
             <v>L*^[H]</v>
           </cell>
           <cell r="B4">
-            <v>98.807000000000002</v>
+            <v>98.281999999999996</v>
           </cell>
           <cell r="C4">
-            <v>1.399</v>
+            <v>1.52</v>
           </cell>
           <cell r="D4">
-            <v>96.066000000000003</v>
+            <v>95.302000000000007</v>
           </cell>
           <cell r="E4">
-            <v>101.548</v>
+            <v>101.261</v>
           </cell>
           <cell r="I4">
-            <v>4.5099999999999998E-14</v>
+            <v>6.7600000000000005E-13</v>
           </cell>
         </row>
         <row r="5">
@@ -11857,19 +11857,19 @@
             <v>^[L*H]</v>
           </cell>
           <cell r="B5">
-            <v>98.397999999999996</v>
+            <v>98.17</v>
           </cell>
           <cell r="C5">
-            <v>1.371</v>
+            <v>1.5649999999999999</v>
           </cell>
           <cell r="D5">
-            <v>95.71</v>
+            <v>95.102000000000004</v>
           </cell>
           <cell r="E5">
-            <v>101.086</v>
+            <v>101.238</v>
           </cell>
           <cell r="I5">
-            <v>2.9899999999999999E-13</v>
+            <v>4.7399999999999999E-14</v>
           </cell>
         </row>
       </sheetData>
@@ -12018,12 +12018,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.93416406076052105</v>
+            <v>0.94231449768906905</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.58258035813071296</v>
+            <v>0.55641710205239003</v>
           </cell>
         </row>
       </sheetData>
@@ -12042,12 +12042,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.89174897721368096</v>
+            <v>0.901950415693481</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.53325993311641395</v>
+            <v>0.46821212674695201</v>
           </cell>
         </row>
       </sheetData>
@@ -12684,23 +12684,23 @@
       </c>
       <c r="B3" s="71">
         <f>[1]LME_PA_l_t_b0!B2</f>
-        <v>93.504000000000005</v>
+        <v>96.254000000000005</v>
       </c>
       <c r="C3" s="77">
         <f>[1]LME_PA_l_t_b0!C2</f>
-        <v>5.6959999999999997</v>
+        <v>5.508</v>
       </c>
       <c r="D3" s="53">
         <f>[1]LME_PA_l_t_b0!D2</f>
-        <v>82.338999999999999</v>
+        <v>85.457999999999998</v>
       </c>
       <c r="E3" s="53">
         <f>[1]LME_PA_l_t_b0!E2</f>
-        <v>104.66800000000001</v>
+        <v>107.04900000000001</v>
       </c>
       <c r="F3" s="54">
         <f>[1]LME_PA_l_t_b0!I2</f>
-        <v>1.11E-7</v>
+        <v>1.37E-8</v>
       </c>
       <c r="H3" s="52" t="str">
         <f>[2]LME_PA_l_f0_b0!A2</f>
@@ -12708,23 +12708,23 @@
       </c>
       <c r="I3" s="69">
         <f>[2]LME_PA_l_f0_b0!B2</f>
-        <v>87.239000000000004</v>
+        <v>86.994</v>
       </c>
       <c r="J3" s="78">
         <f>[2]LME_PA_l_f0_b0!C2</f>
-        <v>1.2709999999999999</v>
+        <v>1.196</v>
       </c>
       <c r="K3" s="78">
         <f>[2]LME_PA_l_f0_b0!D2</f>
-        <v>84.747</v>
+        <v>84.649000000000001</v>
       </c>
       <c r="L3" s="78">
         <f>[2]LME_PA_l_f0_b0!E2</f>
-        <v>89.730999999999995</v>
+        <v>89.337999999999994</v>
       </c>
       <c r="M3" s="54">
         <f>[2]LME_PA_l_f0_b0!I2</f>
-        <v>1.0200000000000001E-12</v>
+        <v>4.1300000000000001E-13</v>
       </c>
       <c r="O3" s="52" t="str">
         <f>[3]LME_PA_f0_exc_b0!A2</f>
@@ -12760,23 +12760,23 @@
       </c>
       <c r="B4" s="71">
         <f>[1]LME_PA_l_t_b0!B3</f>
-        <v>82.188999999999993</v>
+        <v>87.087000000000003</v>
       </c>
       <c r="C4" s="77">
         <f>[1]LME_PA_l_t_b0!C3</f>
-        <v>10.115</v>
+        <v>12.723000000000001</v>
       </c>
       <c r="D4" s="53">
         <f>[1]LME_PA_l_t_b0!D3</f>
-        <v>62.363999999999997</v>
+        <v>62.151000000000003</v>
       </c>
       <c r="E4" s="53">
         <f>[1]LME_PA_l_t_b0!E3</f>
-        <v>102.014</v>
+        <v>112.023</v>
       </c>
       <c r="F4" s="54">
         <f>[1]LME_PA_l_t_b0!I3</f>
-        <v>1.54E-11</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="H4" s="52" t="str">
         <f>[2]LME_PA_l_f0_b0!A3</f>
@@ -12784,23 +12784,23 @@
       </c>
       <c r="I4" s="69">
         <f>[2]LME_PA_l_f0_b0!B3</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="J4" s="78">
         <f>[2]LME_PA_l_f0_b0!C3</f>
-        <v>1.403</v>
+        <v>1.4910000000000001</v>
       </c>
       <c r="K4" s="78">
         <f>[2]LME_PA_l_f0_b0!D3</f>
-        <v>88.575000000000003</v>
+        <v>88.253</v>
       </c>
       <c r="L4" s="78">
         <f>[2]LME_PA_l_f0_b0!E3</f>
-        <v>94.072999999999993</v>
+        <v>94.099000000000004</v>
       </c>
       <c r="M4" s="54">
         <f>[2]LME_PA_l_f0_b0!I3</f>
-        <v>3.0399999999999998E-17</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="O4" s="52" t="str">
         <f>[3]LME_PA_f0_exc_b0!A3</f>
@@ -12836,23 +12836,23 @@
       </c>
       <c r="B5" s="71">
         <f>[1]LME_PA_l_t_b0!B4</f>
-        <v>72.698999999999998</v>
+        <v>73.647000000000006</v>
       </c>
       <c r="C5" s="77">
         <f>[1]LME_PA_l_t_b0!C4</f>
-        <v>6.5590000000000002</v>
+        <v>8.5719999999999992</v>
       </c>
       <c r="D5" s="53">
         <f>[1]LME_PA_l_t_b0!D4</f>
-        <v>59.844000000000001</v>
+        <v>56.845999999999997</v>
       </c>
       <c r="E5" s="53">
         <f>[1]LME_PA_l_t_b0!E4</f>
-        <v>85.552999999999997</v>
+        <v>90.448999999999998</v>
       </c>
       <c r="F5" s="54">
         <f>[1]LME_PA_l_t_b0!I4</f>
-        <v>1.8200000000000001E-8</v>
+        <v>1.45E-4</v>
       </c>
       <c r="H5" s="52" t="str">
         <f>[2]LME_PA_l_f0_b0!A4</f>
@@ -12860,23 +12860,23 @@
       </c>
       <c r="I5" s="69">
         <f>[2]LME_PA_l_f0_b0!B4</f>
-        <v>88.745999999999995</v>
+        <v>88.528999999999996</v>
       </c>
       <c r="J5" s="78">
         <f>[2]LME_PA_l_f0_b0!C4</f>
-        <v>1.292</v>
+        <v>1.2709999999999999</v>
       </c>
       <c r="K5" s="78">
         <f>[2]LME_PA_l_f0_b0!D4</f>
-        <v>86.213999999999999</v>
+        <v>86.037999999999997</v>
       </c>
       <c r="L5" s="78">
         <f>[2]LME_PA_l_f0_b0!E4</f>
-        <v>91.278999999999996</v>
+        <v>91.02</v>
       </c>
       <c r="M5" s="54">
         <f>[2]LME_PA_l_f0_b0!I4</f>
-        <v>2.0399999999999999E-13</v>
+        <v>6.0099999999999996E-13</v>
       </c>
       <c r="O5" s="52" t="str">
         <f>[3]LME_PA_f0_exc_b0!A4</f>
@@ -12912,23 +12912,23 @@
       </c>
       <c r="B6" s="72">
         <f>[1]LME_PA_l_t_b0!B5</f>
-        <v>70.016000000000005</v>
+        <v>69.733999999999995</v>
       </c>
       <c r="C6" s="77">
         <f>[1]LME_PA_l_t_b0!C5</f>
-        <v>5.9580000000000002</v>
+        <v>8.5690000000000008</v>
       </c>
       <c r="D6" s="53">
         <f>[1]LME_PA_l_t_b0!D5</f>
-        <v>58.338000000000001</v>
+        <v>52.939</v>
       </c>
       <c r="E6" s="53">
         <f>[1]LME_PA_l_t_b0!E5</f>
-        <v>81.694000000000003</v>
+        <v>86.528000000000006</v>
       </c>
       <c r="F6" s="56">
         <f>[1]LME_PA_l_t_b0!I5</f>
-        <v>4.6899999999999998E-7</v>
+        <v>6.7500000000000001E-5</v>
       </c>
       <c r="H6" s="55" t="str">
         <f>[2]LME_PA_l_f0_b0!A5</f>
@@ -12936,23 +12936,23 @@
       </c>
       <c r="I6" s="70">
         <f>[2]LME_PA_l_f0_b0!B5</f>
-        <v>91.081999999999994</v>
+        <v>90.988</v>
       </c>
       <c r="J6" s="78">
         <f>[2]LME_PA_l_f0_b0!C5</f>
-        <v>1.2769999999999999</v>
+        <v>1.4179999999999999</v>
       </c>
       <c r="K6" s="78">
         <f>[2]LME_PA_l_f0_b0!D5</f>
-        <v>88.578000000000003</v>
+        <v>88.209000000000003</v>
       </c>
       <c r="L6" s="78">
         <f>[2]LME_PA_l_f0_b0!E5</f>
-        <v>93.585999999999999</v>
+        <v>93.766000000000005</v>
       </c>
       <c r="M6" s="56">
         <f>[2]LME_PA_l_f0_b0!I5</f>
-        <v>4.4800000000000001E-13</v>
+        <v>1.8899999999999999E-15</v>
       </c>
       <c r="O6" s="55" t="str">
         <f>[3]LME_PA_f0_exc_b0!A5</f>
@@ -13112,7 +13112,7 @@
       </c>
       <c r="F10" s="33">
         <f>[4]LME_PA_h_t_b0!I2</f>
-        <v>1.03E-2</v>
+        <v>1.18E-2</v>
       </c>
       <c r="H10" s="61" t="str">
         <f>[5]LME_PA_h_f0_b0!A2</f>
@@ -13120,23 +13120,23 @@
       </c>
       <c r="I10" s="73">
         <f>[5]LME_PA_h_f0_b0!B2</f>
-        <v>93.153000000000006</v>
+        <v>92.605000000000004</v>
       </c>
       <c r="J10" s="79">
         <f>[5]LME_PA_h_f0_b0!C2</f>
-        <v>1.36</v>
+        <v>1.296</v>
       </c>
       <c r="K10" s="79">
         <f>[5]LME_PA_h_f0_b0!D2</f>
-        <v>90.486000000000004</v>
+        <v>90.064999999999998</v>
       </c>
       <c r="L10" s="79">
         <f>[5]LME_PA_h_f0_b0!E2</f>
-        <v>95.819000000000003</v>
+        <v>95.144000000000005</v>
       </c>
       <c r="M10" s="33">
         <f>[5]LME_PA_h_f0_b0!I2</f>
-        <v>1.0200000000000001E-12</v>
+        <v>5.6500000000000002E-13</v>
       </c>
       <c r="O10" s="61" t="str">
         <f>[6]LME_PA_lh_slope_b0!A2</f>
@@ -13191,7 +13191,7 @@
       </c>
       <c r="F11" s="33">
         <f>[4]LME_PA_h_t_b0!I3</f>
-        <v>5.8999999999999999E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="H11" s="61" t="str">
         <f>[5]LME_PA_h_f0_b0!A3</f>
@@ -13199,23 +13199,23 @@
       </c>
       <c r="I11" s="73">
         <f>[5]LME_PA_h_f0_b0!B3</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="J11" s="79">
         <f>[5]LME_PA_h_f0_b0!C3</f>
-        <v>1.5960000000000001</v>
+        <v>1.7789999999999999</v>
       </c>
       <c r="K11" s="79">
         <f>[5]LME_PA_h_f0_b0!D3</f>
-        <v>91.39</v>
+        <v>90.406000000000006</v>
       </c>
       <c r="L11" s="79">
         <f>[5]LME_PA_h_f0_b0!E3</f>
-        <v>97.647999999999996</v>
+        <v>97.379000000000005</v>
       </c>
       <c r="M11" s="33">
         <f>[5]LME_PA_h_f0_b0!I3</f>
-        <v>2.42E-20</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="O11" s="61" t="str">
         <f>[6]LME_PA_lh_slope_b0!A3</f>
@@ -13265,7 +13265,7 @@
       </c>
       <c r="F12" s="33">
         <f>[4]LME_PA_h_t_b0!I4</f>
-        <v>9.1000000000000004E-3</v>
+        <v>1.04E-2</v>
       </c>
       <c r="H12" s="61" t="str">
         <f>[5]LME_PA_h_f0_b0!A4</f>
@@ -13273,23 +13273,23 @@
       </c>
       <c r="I12" s="73">
         <f>[5]LME_PA_h_f0_b0!B4</f>
-        <v>98.807000000000002</v>
+        <v>98.281999999999996</v>
       </c>
       <c r="J12" s="79">
         <f>[5]LME_PA_h_f0_b0!C4</f>
-        <v>1.399</v>
+        <v>1.52</v>
       </c>
       <c r="K12" s="79">
         <f>[5]LME_PA_h_f0_b0!D4</f>
-        <v>96.066000000000003</v>
+        <v>95.302000000000007</v>
       </c>
       <c r="L12" s="79">
         <f>[5]LME_PA_h_f0_b0!E4</f>
-        <v>101.548</v>
+        <v>101.261</v>
       </c>
       <c r="M12" s="33">
         <f>[5]LME_PA_h_f0_b0!I4</f>
-        <v>4.5099999999999998E-14</v>
+        <v>6.7600000000000005E-13</v>
       </c>
       <c r="O12" s="61" t="str">
         <f>[6]LME_PA_lh_slope_b0!A4</f>
@@ -13339,7 +13339,7 @@
       </c>
       <c r="F13" s="35">
         <f>[4]LME_PA_h_t_b0!I5</f>
-        <v>1.12E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="H13" s="63" t="str">
         <f>[5]LME_PA_h_f0_b0!A5</f>
@@ -13347,23 +13347,23 @@
       </c>
       <c r="I13" s="74">
         <f>[5]LME_PA_h_f0_b0!B5</f>
-        <v>98.397999999999996</v>
+        <v>98.17</v>
       </c>
       <c r="J13" s="79">
         <f>[5]LME_PA_h_f0_b0!C5</f>
-        <v>1.371</v>
+        <v>1.5649999999999999</v>
       </c>
       <c r="K13" s="79">
         <f>[5]LME_PA_h_f0_b0!D5</f>
-        <v>95.71</v>
+        <v>95.102000000000004</v>
       </c>
       <c r="L13" s="79">
         <f>[5]LME_PA_h_f0_b0!E5</f>
-        <v>101.086</v>
+        <v>101.238</v>
       </c>
       <c r="M13" s="35">
         <f>[5]LME_PA_h_f0_b0!I5</f>
-        <v>2.9899999999999999E-13</v>
+        <v>4.7399999999999999E-14</v>
       </c>
       <c r="O13" s="63" t="str">
         <f>[6]LME_PA_lh_slope_b0!A5</f>
@@ -13713,101 +13713,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="80" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="156" t="s">
+      <c r="B1" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="157"/>
-      <c r="I1" s="157"/>
-      <c r="J1" s="157"/>
-      <c r="K1" s="157"/>
-      <c r="L1" s="157"/>
-      <c r="M1" s="157"/>
-      <c r="N1" s="157"/>
-      <c r="O1" s="157"/>
-      <c r="P1" s="157"/>
-      <c r="Q1" s="157"/>
-      <c r="R1" s="157"/>
-      <c r="S1" s="157"/>
-      <c r="T1" s="157"/>
-      <c r="U1" s="157"/>
-      <c r="V1" s="157"/>
-      <c r="W1" s="157"/>
-      <c r="X1" s="157"/>
-      <c r="Y1" s="157"/>
-      <c r="Z1" s="157"/>
-      <c r="AA1" s="157"/>
-      <c r="AB1" s="157"/>
-      <c r="AC1" s="157"/>
-      <c r="AD1" s="157"/>
-      <c r="AE1" s="157"/>
-      <c r="AF1" s="157"/>
-      <c r="AG1" s="158"/>
-      <c r="AH1" s="147" t="s">
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="161"/>
+      <c r="M1" s="161"/>
+      <c r="N1" s="161"/>
+      <c r="O1" s="161"/>
+      <c r="P1" s="161"/>
+      <c r="Q1" s="161"/>
+      <c r="R1" s="161"/>
+      <c r="S1" s="161"/>
+      <c r="T1" s="161"/>
+      <c r="U1" s="161"/>
+      <c r="V1" s="161"/>
+      <c r="W1" s="161"/>
+      <c r="X1" s="161"/>
+      <c r="Y1" s="161"/>
+      <c r="Z1" s="161"/>
+      <c r="AA1" s="161"/>
+      <c r="AB1" s="161"/>
+      <c r="AC1" s="161"/>
+      <c r="AD1" s="161"/>
+      <c r="AE1" s="161"/>
+      <c r="AF1" s="161"/>
+      <c r="AG1" s="162"/>
+      <c r="AH1" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="148"/>
+      <c r="AI1" s="152"/>
     </row>
     <row r="2" spans="1:35" s="81" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="152"/>
-      <c r="B2" s="153" t="str">
+      <c r="A2" s="156"/>
+      <c r="B2" s="157" t="str">
         <f>Intercepts!A3</f>
         <v>L*H</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="153" t="str">
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="157" t="str">
         <f>Intercepts!A4</f>
         <v>^[L*]H</v>
       </c>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="153" t="str">
+      <c r="K2" s="158"/>
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="157" t="str">
         <f>Intercepts!A5</f>
         <v>L*^[H]</v>
       </c>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="154"/>
-      <c r="X2" s="154"/>
-      <c r="Y2" s="155"/>
-      <c r="Z2" s="153" t="str">
+      <c r="S2" s="158"/>
+      <c r="T2" s="158"/>
+      <c r="U2" s="158"/>
+      <c r="V2" s="158"/>
+      <c r="W2" s="158"/>
+      <c r="X2" s="158"/>
+      <c r="Y2" s="159"/>
+      <c r="Z2" s="157" t="str">
         <f>Intercepts!A6</f>
         <v>^[L*H]</v>
       </c>
-      <c r="AA2" s="154"/>
-      <c r="AB2" s="154"/>
-      <c r="AC2" s="154"/>
-      <c r="AD2" s="154"/>
-      <c r="AE2" s="154"/>
-      <c r="AF2" s="154"/>
-      <c r="AG2" s="155"/>
-      <c r="AH2" s="149" t="s">
+      <c r="AA2" s="158"/>
+      <c r="AB2" s="158"/>
+      <c r="AC2" s="158"/>
+      <c r="AD2" s="158"/>
+      <c r="AE2" s="158"/>
+      <c r="AF2" s="158"/>
+      <c r="AG2" s="159"/>
+      <c r="AH2" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="AI2" s="150"/>
+      <c r="AI2" s="154"/>
     </row>
     <row r="3" spans="1:35" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="148" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="83" t="s">
@@ -13943,139 +13943,139 @@
       </c>
       <c r="B4" s="91">
         <f>[2]LME_PA_l_f0_b0!B2</f>
-        <v>87.239000000000004</v>
+        <v>86.994</v>
       </c>
       <c r="C4" s="92">
         <f>[2]LME_PA_l_f0_b0!C2</f>
-        <v>1.2709999999999999</v>
+        <v>1.196</v>
       </c>
       <c r="D4" s="93">
         <f>[2]LME_PA_l_f0_b0!D2</f>
-        <v>84.747</v>
+        <v>84.649000000000001</v>
       </c>
       <c r="E4" s="93">
         <f>[2]LME_PA_l_f0_b0!E2</f>
-        <v>89.730999999999995</v>
+        <v>89.337999999999994</v>
       </c>
       <c r="F4" s="92">
         <f>[2]LME_PA_l_f0_b0!F2</f>
-        <v>68.623000000000005</v>
+        <v>72.718999999999994</v>
       </c>
       <c r="G4" s="92">
         <f>[2]LME_PA_l_f0_b0!G2</f>
-        <v>9.01</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H4" s="94">
         <f>[2]LME_PA_l_f0_b0!H2</f>
-        <v>1.4600000000000001E-13</v>
+        <v>5.1600000000000002E-14</v>
       </c>
       <c r="I4" s="95">
         <f>[2]LME_PA_l_f0_b0!I2</f>
-        <v>1.0200000000000001E-12</v>
+        <v>4.1300000000000001E-13</v>
       </c>
       <c r="J4" s="96">
         <f>[2]LME_PA_l_f0_b0!B3</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="K4" s="92">
         <f>[2]LME_PA_l_f0_b0!C3</f>
-        <v>1.403</v>
+        <v>1.4910000000000001</v>
       </c>
       <c r="L4" s="93">
         <f>[2]LME_PA_l_f0_b0!D3</f>
-        <v>88.575000000000003</v>
+        <v>88.253</v>
       </c>
       <c r="M4" s="93">
         <f>[2]LME_PA_l_f0_b0!E3</f>
-        <v>94.072999999999993</v>
+        <v>94.099000000000004</v>
       </c>
       <c r="N4" s="92">
         <f>[2]LME_PA_l_f0_b0!F3</f>
-        <v>65.114000000000004</v>
+        <v>61.14</v>
       </c>
       <c r="O4" s="92">
         <f>[2]LME_PA_l_f0_b0!G3</f>
-        <v>13.34</v>
+        <v>0</v>
       </c>
       <c r="P4" s="97">
         <f>[2]LME_PA_l_f0_b0!H3</f>
-        <v>4.34E-18</v>
+        <v>0.99970000000000003</v>
       </c>
       <c r="Q4" s="98">
         <f>[2]LME_PA_l_f0_b0!I3</f>
-        <v>3.0399999999999998E-17</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="R4" s="96">
         <f>[2]LME_PA_l_f0_b0!B3</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="S4" s="92">
         <f>[2]LME_PA_l_f0_b0!C3</f>
-        <v>1.403</v>
+        <v>1.4910000000000001</v>
       </c>
       <c r="T4" s="93">
         <f>[2]LME_PA_l_f0_b0!D3</f>
-        <v>88.575000000000003</v>
+        <v>88.253</v>
       </c>
       <c r="U4" s="93">
         <f>[2]LME_PA_l_f0_b0!E3</f>
-        <v>94.072999999999993</v>
+        <v>94.099000000000004</v>
       </c>
       <c r="V4" s="92">
         <f>[2]LME_PA_l_f0_b0!F3</f>
-        <v>65.114000000000004</v>
+        <v>61.14</v>
       </c>
       <c r="W4" s="92">
         <f>[2]LME_PA_l_f0_b0!G3</f>
-        <v>13.34</v>
+        <v>0</v>
       </c>
       <c r="X4" s="97">
         <f>[2]LME_PA_l_f0_b0!H3</f>
-        <v>4.34E-18</v>
+        <v>0.99970000000000003</v>
       </c>
       <c r="Y4" s="98">
         <f>[2]LME_PA_l_f0_b0!I3</f>
-        <v>3.0399999999999998E-17</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="Z4" s="93">
         <f>[2]LME_PA_l_f0_b0!B3</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="AA4" s="93">
         <f>[2]LME_PA_l_f0_b0!C3</f>
-        <v>1.403</v>
+        <v>1.4910000000000001</v>
       </c>
       <c r="AB4" s="93">
         <f>[2]LME_PA_l_f0_b0!D3</f>
-        <v>88.575000000000003</v>
+        <v>88.253</v>
       </c>
       <c r="AC4" s="93">
         <f>[2]LME_PA_l_f0_b0!E3</f>
-        <v>94.072999999999993</v>
+        <v>94.099000000000004</v>
       </c>
       <c r="AD4" s="92">
         <f>[2]LME_PA_l_f0_b0!F3</f>
-        <v>65.114000000000004</v>
+        <v>61.14</v>
       </c>
       <c r="AE4" s="92">
         <f>[2]LME_PA_l_f0_b0!G3</f>
-        <v>13.34</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="97">
         <f>[2]LME_PA_l_f0_b0!H3</f>
-        <v>4.34E-18</v>
+        <v>0.99970000000000003</v>
       </c>
       <c r="AG4" s="98">
         <f>[2]LME_PA_l_f0_b0!I3</f>
-        <v>3.0399999999999998E-17</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AH4" s="99">
         <f>[7]LME_PA_l_f0_r2!$B$3</f>
-        <v>0.58258035813071296</v>
+        <v>0.55641710205239003</v>
       </c>
       <c r="AI4" s="100">
         <f>[7]LME_PA_l_f0_r2!$B$2</f>
-        <v>0.93416406076052105</v>
+        <v>0.94231449768906905</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="101" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -14084,143 +14084,143 @@
       </c>
       <c r="B5" s="103">
         <f>[5]LME_PA_h_f0_b0!B2</f>
-        <v>93.153000000000006</v>
+        <v>92.605000000000004</v>
       </c>
       <c r="C5" s="104">
         <f>[5]LME_PA_h_f0_b0!C2</f>
-        <v>1.36</v>
+        <v>1.296</v>
       </c>
       <c r="D5" s="105">
         <f>[5]LME_PA_h_f0_b0!D2</f>
-        <v>90.486000000000004</v>
+        <v>90.064999999999998</v>
       </c>
       <c r="E5" s="105">
         <f>[5]LME_PA_h_f0_b0!E2</f>
-        <v>95.819000000000003</v>
+        <v>95.144000000000005</v>
       </c>
       <c r="F5" s="104">
         <f>[5]LME_PA_h_f0_b0!F2</f>
-        <v>68.471999999999994</v>
+        <v>71.475999999999999</v>
       </c>
       <c r="G5" s="104">
         <f>[5]LME_PA_h_f0_b0!G2</f>
-        <v>9.02</v>
+        <v>9.14</v>
       </c>
       <c r="H5" s="106">
         <f>[5]LME_PA_h_f0_b0!H2</f>
-        <v>1.4499999999999999E-13</v>
+        <v>7.0700000000000004E-14</v>
       </c>
       <c r="I5" s="107">
         <f>[5]LME_PA_h_f0_b0!I2</f>
-        <v>1.0200000000000001E-12</v>
+        <v>5.6500000000000002E-13</v>
       </c>
       <c r="J5" s="108">
         <f>[5]LME_PA_h_f0_b0!B3</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="K5" s="104">
         <f>[5]LME_PA_h_f0_b0!C3</f>
-        <v>1.5960000000000001</v>
+        <v>1.7789999999999999</v>
       </c>
       <c r="L5" s="105">
         <f>[5]LME_PA_h_f0_b0!D3</f>
-        <v>91.39</v>
+        <v>90.406000000000006</v>
       </c>
       <c r="M5" s="105">
         <f>[5]LME_PA_h_f0_b0!E3</f>
-        <v>97.647999999999996</v>
+        <v>97.379000000000005</v>
       </c>
       <c r="N5" s="104">
         <f>[5]LME_PA_h_f0_b0!F3</f>
-        <v>59.206000000000003</v>
+        <v>52.786999999999999</v>
       </c>
       <c r="O5" s="104">
         <f>[5]LME_PA_h_f0_b0!G3</f>
-        <v>17.059999999999999</v>
+        <v>0</v>
       </c>
       <c r="P5" s="106">
         <f>[5]LME_PA_h_f0_b0!H3</f>
-        <v>3.4500000000000002E-21</v>
+        <v>0.99439999999999995</v>
       </c>
       <c r="Q5" s="107">
         <f>[5]LME_PA_h_f0_b0!I3</f>
-        <v>2.42E-20</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="R5" s="108">
         <f>[5]LME_PA_h_f0_b0!B3</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="S5" s="104">
         <f>[5]LME_PA_h_f0_b0!C3</f>
-        <v>1.5960000000000001</v>
+        <v>1.7789999999999999</v>
       </c>
       <c r="T5" s="105">
         <f>[5]LME_PA_h_f0_b0!D3</f>
-        <v>91.39</v>
+        <v>90.406000000000006</v>
       </c>
       <c r="U5" s="105">
         <f>[5]LME_PA_h_f0_b0!E3</f>
-        <v>97.647999999999996</v>
+        <v>97.379000000000005</v>
       </c>
       <c r="V5" s="104">
         <f>[5]LME_PA_h_f0_b0!F3</f>
-        <v>59.206000000000003</v>
+        <v>52.786999999999999</v>
       </c>
       <c r="W5" s="104">
         <f>[5]LME_PA_h_f0_b0!G3</f>
-        <v>17.059999999999999</v>
+        <v>0</v>
       </c>
       <c r="X5" s="106">
         <f>[5]LME_PA_h_f0_b0!H3</f>
-        <v>3.4500000000000002E-21</v>
+        <v>0.99439999999999995</v>
       </c>
       <c r="Y5" s="107">
         <f>[5]LME_PA_h_f0_b0!I3</f>
-        <v>2.42E-20</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="Z5" s="105">
         <f>[5]LME_PA_h_f0_b0!B3</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="AA5" s="105">
         <f>[5]LME_PA_h_f0_b0!C3</f>
-        <v>1.5960000000000001</v>
+        <v>1.7789999999999999</v>
       </c>
       <c r="AB5" s="105">
         <f>[5]LME_PA_h_f0_b0!D3</f>
-        <v>91.39</v>
+        <v>90.406000000000006</v>
       </c>
       <c r="AC5" s="105">
         <f>[5]LME_PA_h_f0_b0!E3</f>
-        <v>97.647999999999996</v>
+        <v>97.379000000000005</v>
       </c>
       <c r="AD5" s="104">
         <f>[5]LME_PA_h_f0_b0!F3</f>
-        <v>59.206000000000003</v>
+        <v>52.786999999999999</v>
       </c>
       <c r="AE5" s="104">
         <f>[5]LME_PA_h_f0_b0!G3</f>
-        <v>17.059999999999999</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="106">
         <f>[5]LME_PA_h_f0_b0!H3</f>
-        <v>3.4500000000000002E-21</v>
+        <v>0.99439999999999995</v>
       </c>
       <c r="AG5" s="107">
         <f>[5]LME_PA_h_f0_b0!I3</f>
-        <v>2.42E-20</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AH5" s="109">
         <f>[8]LME_PA_h_f0_r2!$B$3</f>
-        <v>0.53325993311641395</v>
+        <v>0.46821212674695201</v>
       </c>
       <c r="AI5" s="110">
         <f>[8]LME_PA_h_f0_r2!$B$2</f>
-        <v>0.89174897721368096</v>
+        <v>0.901950415693481</v>
       </c>
     </row>
     <row r="6" spans="1:35" s="101" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="147" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="103">
@@ -14361,7 +14361,7 @@
       </c>
     </row>
     <row r="7" spans="1:35" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="148" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="83" t="str">
@@ -14505,143 +14505,143 @@
       </c>
       <c r="B8" s="114">
         <f>[1]LME_PA_l_t_b0!B2</f>
-        <v>93.504000000000005</v>
+        <v>96.254000000000005</v>
       </c>
       <c r="C8" s="115">
         <f>[1]LME_PA_l_t_b0!C2</f>
-        <v>5.6959999999999997</v>
+        <v>5.508</v>
       </c>
       <c r="D8" s="115">
         <f>[1]LME_PA_l_t_b0!D2</f>
-        <v>82.338999999999999</v>
+        <v>85.457999999999998</v>
       </c>
       <c r="E8" s="115">
         <f>[1]LME_PA_l_t_b0!E2</f>
-        <v>104.66800000000001</v>
+        <v>107.04900000000001</v>
       </c>
       <c r="F8" s="116">
         <f>[1]LME_PA_l_t_b0!F2</f>
-        <v>16.414999999999999</v>
+        <v>17.475000000000001</v>
       </c>
       <c r="G8" s="116">
         <f>[1]LME_PA_l_t_b0!G2</f>
-        <v>9.94</v>
+        <v>11.23</v>
       </c>
       <c r="H8" s="97">
         <f>[1]LME_PA_l_t_b0!H2</f>
-        <v>1.5799999999999999E-8</v>
+        <v>1.7100000000000001E-9</v>
       </c>
       <c r="I8" s="98">
         <f>[1]LME_PA_l_t_b0!I2</f>
-        <v>1.11E-7</v>
+        <v>1.37E-8</v>
       </c>
       <c r="J8" s="117">
         <f>[1]LME_PA_l_t_b0!B3</f>
-        <v>82.188999999999993</v>
+        <v>87.087000000000003</v>
       </c>
       <c r="K8" s="116">
         <f>[1]LME_PA_l_t_b0!C3</f>
-        <v>10.115</v>
+        <v>12.723000000000001</v>
       </c>
       <c r="L8" s="118">
         <f>[1]LME_PA_l_t_b0!D3</f>
-        <v>62.363999999999997</v>
+        <v>62.151000000000003</v>
       </c>
       <c r="M8" s="118">
         <f>[1]LME_PA_l_t_b0!E3</f>
-        <v>102.014</v>
+        <v>112.023</v>
       </c>
       <c r="N8" s="116">
         <f>[1]LME_PA_l_t_b0!F3</f>
-        <v>8.1259999999999994</v>
+        <v>6.8449999999999998</v>
       </c>
       <c r="O8" s="116">
         <f>[1]LME_PA_l_t_b0!G3</f>
-        <v>90.27</v>
+        <v>0</v>
       </c>
       <c r="P8" s="97">
         <f>[1]LME_PA_l_t_b0!H3</f>
-        <v>2.2100000000000001E-12</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="98">
         <f>[1]LME_PA_l_t_b0!I3</f>
-        <v>1.54E-11</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="R8" s="117">
         <f>[1]LME_PA_l_t_b0!B4</f>
-        <v>72.698999999999998</v>
+        <v>73.647000000000006</v>
       </c>
       <c r="S8" s="116">
         <f>[1]LME_PA_l_t_b0!C4</f>
-        <v>6.5590000000000002</v>
+        <v>8.5719999999999992</v>
       </c>
       <c r="T8" s="118">
         <f>[1]LME_PA_l_t_b0!D4</f>
-        <v>59.844000000000001</v>
+        <v>56.845999999999997</v>
       </c>
       <c r="U8" s="118">
         <f>[1]LME_PA_l_t_b0!E4</f>
-        <v>85.552999999999997</v>
+        <v>90.448999999999998</v>
       </c>
       <c r="V8" s="116">
         <f>[1]LME_PA_l_t_b0!F4</f>
-        <v>11.084</v>
+        <v>8.5909999999999993</v>
       </c>
       <c r="W8" s="116">
         <f>[1]LME_PA_l_t_b0!G4</f>
-        <v>17.399999999999999</v>
+        <v>8.49</v>
       </c>
       <c r="X8" s="97">
         <f>[1]LME_PA_l_t_b0!H4</f>
-        <v>2.6000000000000001E-9</v>
+        <v>1.8099999999999999E-5</v>
       </c>
       <c r="Y8" s="98">
         <f>[1]LME_PA_l_t_b0!I4</f>
-        <v>1.8200000000000001E-8</v>
+        <v>1.45E-4</v>
       </c>
       <c r="Z8" s="118">
         <f>[1]LME_PA_l_t_b0!B5</f>
-        <v>70.016000000000005</v>
+        <v>69.733999999999995</v>
       </c>
       <c r="AA8" s="118">
         <f>[1]LME_PA_l_t_b0!C5</f>
-        <v>5.9580000000000002</v>
+        <v>8.5690000000000008</v>
       </c>
       <c r="AB8" s="118">
         <f>[1]LME_PA_l_t_b0!D5</f>
-        <v>58.338000000000001</v>
+        <v>52.939</v>
       </c>
       <c r="AC8" s="118">
         <f>[1]LME_PA_l_t_b0!E5</f>
-        <v>81.694000000000003</v>
+        <v>86.528000000000006</v>
       </c>
       <c r="AD8" s="116">
         <f>[1]LME_PA_l_t_b0!F5</f>
-        <v>11.750999999999999</v>
+        <v>8.1379999999999999</v>
       </c>
       <c r="AE8" s="116">
         <f>[1]LME_PA_l_t_b0!G5</f>
-        <v>11.89</v>
+        <v>10.3</v>
       </c>
       <c r="AF8" s="97">
         <f>[1]LME_PA_l_t_b0!H5</f>
-        <v>6.6899999999999997E-8</v>
+        <v>8.4400000000000005E-6</v>
       </c>
       <c r="AG8" s="98">
         <f>[1]LME_PA_l_t_b0!I5</f>
-        <v>4.6899999999999998E-7</v>
+        <v>6.7500000000000001E-5</v>
       </c>
       <c r="AH8" s="119">
         <f>[10]LME_PA_l_t_r2!$B$3</f>
-        <v>0.593435532261537</v>
+        <v>0.62408082900844397</v>
       </c>
       <c r="AI8" s="120">
         <f>[10]LME_PA_l_t_r2!$B$2</f>
-        <v>0.73093594252433203</v>
+        <v>0.80115699175044897</v>
       </c>
     </row>
     <row r="9" spans="1:35" s="121" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="165" t="s">
+      <c r="A9" s="149" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="122">
@@ -14674,7 +14674,7 @@
       </c>
       <c r="I9" s="107">
         <f>[4]LME_PA_h_t_b0!I2</f>
-        <v>1.03E-2</v>
+        <v>1.18E-2</v>
       </c>
       <c r="J9" s="124">
         <f>[4]LME_PA_h_t_b0!B3</f>
@@ -14706,7 +14706,7 @@
       </c>
       <c r="Q9" s="107">
         <f>[4]LME_PA_h_t_b0!I3</f>
-        <v>5.8999999999999999E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="R9" s="124">
         <f>[4]LME_PA_h_t_b0!B4</f>
@@ -14738,7 +14738,7 @@
       </c>
       <c r="Y9" s="107">
         <f>[4]LME_PA_h_t_b0!I4</f>
-        <v>9.1000000000000004E-3</v>
+        <v>1.04E-2</v>
       </c>
       <c r="Z9" s="105">
         <f>[4]LME_PA_h_t_b0!B5</f>
@@ -14770,7 +14770,7 @@
       </c>
       <c r="AG9" s="107">
         <f>[4]LME_PA_h_t_b0!I5</f>
-        <v>1.12E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="AH9" s="109">
         <f>[11]LME_PA_h_t_r2!$B$3</f>
@@ -14782,7 +14782,7 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="148" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="83" t="str">
@@ -14921,7 +14921,7 @@
       </c>
     </row>
     <row r="11" spans="1:35" s="101" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="150" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="125">
@@ -15513,72 +15513,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="80" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="162" t="s">
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="162"/>
-      <c r="AH1" s="162"/>
-      <c r="AI1" s="162"/>
-      <c r="AJ1" s="162"/>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="162"/>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="162"/>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
-      <c r="AZ1" s="162"/>
-      <c r="BA1" s="162"/>
-      <c r="BB1" s="147" t="s">
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
+      <c r="I1" s="164"/>
+      <c r="J1" s="164"/>
+      <c r="K1" s="164"/>
+      <c r="L1" s="164"/>
+      <c r="M1" s="164"/>
+      <c r="N1" s="164"/>
+      <c r="O1" s="164"/>
+      <c r="P1" s="164"/>
+      <c r="Q1" s="164"/>
+      <c r="R1" s="164"/>
+      <c r="S1" s="164"/>
+      <c r="T1" s="164"/>
+      <c r="U1" s="164"/>
+      <c r="V1" s="164"/>
+      <c r="W1" s="164"/>
+      <c r="X1" s="164"/>
+      <c r="Y1" s="164"/>
+      <c r="Z1" s="164"/>
+      <c r="AA1" s="164"/>
+      <c r="AB1" s="164"/>
+      <c r="AC1" s="164"/>
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
+      <c r="AV1" s="164"/>
+      <c r="AW1" s="164"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
+      <c r="AZ1" s="164"/>
+      <c r="BA1" s="164"/>
+      <c r="BB1" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="BC1" s="148"/>
+      <c r="BC1" s="152"/>
     </row>
     <row r="2" spans="1:55" s="81" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="152"/>
+      <c r="A2" s="156"/>
       <c r="B2" s="137" t="str">
         <f>Intercepts!A3</f>
         <v>L*H</v>
@@ -15595,76 +15595,76 @@
         <f>Intercepts!A6</f>
         <v>^[L*H]</v>
       </c>
-      <c r="F2" s="149" t="str">
+      <c r="F2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A2, " vs ", [13]LME_PA_f0_exc_b1!B2)</f>
         <v>L*H vs ^[L*]H</v>
       </c>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
-      <c r="L2" s="160"/>
-      <c r="M2" s="150"/>
-      <c r="N2" s="149" t="str">
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A3, " vs ", [13]LME_PA_f0_exc_b1!B3)</f>
         <v>L*H vs L*^[H]</v>
       </c>
-      <c r="O2" s="159"/>
-      <c r="P2" s="159"/>
-      <c r="Q2" s="160"/>
-      <c r="R2" s="160"/>
-      <c r="S2" s="160"/>
-      <c r="T2" s="160"/>
-      <c r="U2" s="150"/>
-      <c r="V2" s="149" t="str">
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="166"/>
+      <c r="R2" s="166"/>
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="154"/>
+      <c r="V2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A4, " vs ", [13]LME_PA_f0_exc_b1!B4)</f>
         <v>L*H vs ^[L*H]</v>
       </c>
-      <c r="W2" s="159"/>
-      <c r="X2" s="159"/>
-      <c r="Y2" s="160"/>
-      <c r="Z2" s="160"/>
-      <c r="AA2" s="160"/>
-      <c r="AB2" s="160"/>
-      <c r="AC2" s="150"/>
-      <c r="AD2" s="149" t="str">
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="166"/>
+      <c r="Z2" s="166"/>
+      <c r="AA2" s="166"/>
+      <c r="AB2" s="166"/>
+      <c r="AC2" s="154"/>
+      <c r="AD2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A5, " vs ", [13]LME_PA_f0_exc_b1!B5)</f>
         <v>^[L*]H vs L*^[H]</v>
       </c>
-      <c r="AE2" s="159"/>
-      <c r="AF2" s="159"/>
-      <c r="AG2" s="160"/>
-      <c r="AH2" s="160"/>
-      <c r="AI2" s="160"/>
-      <c r="AJ2" s="160"/>
-      <c r="AK2" s="150"/>
-      <c r="AL2" s="149" t="str">
+      <c r="AE2" s="165"/>
+      <c r="AF2" s="165"/>
+      <c r="AG2" s="166"/>
+      <c r="AH2" s="166"/>
+      <c r="AI2" s="166"/>
+      <c r="AJ2" s="166"/>
+      <c r="AK2" s="154"/>
+      <c r="AL2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A6, " vs ", [13]LME_PA_f0_exc_b1!B6)</f>
         <v>^[L*]H vs ^[L*H]</v>
       </c>
-      <c r="AM2" s="159"/>
-      <c r="AN2" s="159"/>
-      <c r="AO2" s="160"/>
-      <c r="AP2" s="160"/>
-      <c r="AQ2" s="160"/>
-      <c r="AR2" s="160"/>
-      <c r="AS2" s="150"/>
-      <c r="AT2" s="149" t="str">
+      <c r="AM2" s="165"/>
+      <c r="AN2" s="165"/>
+      <c r="AO2" s="166"/>
+      <c r="AP2" s="166"/>
+      <c r="AQ2" s="166"/>
+      <c r="AR2" s="166"/>
+      <c r="AS2" s="154"/>
+      <c r="AT2" s="153" t="str">
         <f>_xlfn.CONCAT([13]LME_PA_f0_exc_b1!A7, " vs ", [13]LME_PA_f0_exc_b1!B7)</f>
         <v>L*^[H] vs ^[L*H]</v>
       </c>
-      <c r="AU2" s="159"/>
-      <c r="AV2" s="159"/>
-      <c r="AW2" s="160"/>
-      <c r="AX2" s="160"/>
-      <c r="AY2" s="160"/>
-      <c r="AZ2" s="160"/>
-      <c r="BA2" s="150"/>
-      <c r="BB2" s="149" t="s">
+      <c r="AU2" s="165"/>
+      <c r="AV2" s="165"/>
+      <c r="AW2" s="166"/>
+      <c r="AX2" s="166"/>
+      <c r="AY2" s="166"/>
+      <c r="AZ2" s="166"/>
+      <c r="BA2" s="154"/>
+      <c r="BB2" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="BC2" s="150"/>
+      <c r="BC2" s="154"/>
     </row>
     <row r="3" spans="1:55" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="82" t="s">
@@ -15879,175 +15879,175 @@
       </c>
       <c r="B4" s="91">
         <f>Intercepts!I3</f>
-        <v>87.239000000000004</v>
+        <v>86.994</v>
       </c>
       <c r="C4" s="96">
         <f>Intercepts!I4</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="D4" s="96">
         <f>Intercepts!I5</f>
-        <v>88.745999999999995</v>
+        <v>88.528999999999996</v>
       </c>
       <c r="E4" s="140">
         <f>Intercepts!I6</f>
-        <v>91.081999999999994</v>
+        <v>90.988</v>
       </c>
       <c r="F4" s="99">
         <f>[14]LME_PA_l_f0_b1!C2</f>
-        <v>4.085</v>
+        <v>4.3390000000000004</v>
       </c>
       <c r="G4" s="92">
         <f>[14]LME_PA_l_f0_b1!D2</f>
-        <v>0.58599999999999997</v>
+        <v>1.3</v>
       </c>
       <c r="H4" s="93">
         <f>[14]LME_PA_l_f0_b1!E2</f>
-        <v>2.9359999999999999</v>
+        <v>1.79</v>
       </c>
       <c r="I4" s="93">
         <f>[14]LME_PA_l_f0_b1!F2</f>
-        <v>5.2350000000000003</v>
+        <v>6.8879999999999999</v>
       </c>
       <c r="J4" s="92">
         <f>[14]LME_PA_l_f0_b1!G2</f>
-        <v>6.9660000000000002</v>
+        <v>3.3370000000000002</v>
       </c>
       <c r="K4" s="92">
         <f>[14]LME_PA_l_f0_b1!H2</f>
-        <v>613.48</v>
+        <v>1.94</v>
       </c>
       <c r="L4" s="94">
         <f>[14]LME_PA_l_f0_b1!I2</f>
-        <v>8.4099999999999999E-12</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="M4" s="95">
         <f>[14]LME_PA_l_f0_b1!J2</f>
-        <v>5.8899999999999998E-11</v>
+        <v>0.6603</v>
       </c>
       <c r="N4" s="99">
         <f>[14]LME_PA_l_f0_b1!C3</f>
-        <v>1.5069999999999999</v>
+        <v>1.536</v>
       </c>
       <c r="O4" s="92">
         <f>[14]LME_PA_l_f0_b1!D3</f>
-        <v>0.251</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="P4" s="93">
         <f>[14]LME_PA_l_f0_b1!E3</f>
-        <v>1.0149999999999999</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="Q4" s="93">
         <f>[14]LME_PA_l_f0_b1!F3</f>
-        <v>2</v>
+        <v>2.3559999999999999</v>
       </c>
       <c r="R4" s="92">
         <f>[14]LME_PA_l_f0_b1!G3</f>
-        <v>6.0039999999999996</v>
+        <v>3.6680000000000001</v>
       </c>
       <c r="S4" s="92">
         <f>[14]LME_PA_l_f0_b1!H3</f>
-        <v>613.33000000000004</v>
+        <v>1.73</v>
       </c>
       <c r="T4" s="94">
         <f>[14]LME_PA_l_f0_b1!I3</f>
-        <v>3.3000000000000002E-9</v>
+        <v>8.2600000000000007E-2</v>
       </c>
       <c r="U4" s="95">
         <f>[14]LME_PA_l_f0_b1!I3</f>
-        <v>3.3000000000000002E-9</v>
+        <v>8.2600000000000007E-2</v>
       </c>
       <c r="V4" s="99">
         <f>[14]LME_PA_l_f0_b1!C4</f>
-        <v>3.843</v>
+        <v>3.9940000000000002</v>
       </c>
       <c r="W4" s="92">
         <f>[14]LME_PA_l_f0_b1!D4</f>
-        <v>0.14099999999999999</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="X4" s="93">
         <f>[14]LME_PA_l_f0_b1!E4</f>
-        <v>3.5659999999999998</v>
+        <v>2.7890000000000001</v>
       </c>
       <c r="Y4" s="93">
         <f>[14]LME_PA_l_f0_b1!F4</f>
-        <v>4.12</v>
+        <v>5.1989999999999998</v>
       </c>
       <c r="Z4" s="92">
         <f>[14]LME_PA_l_f0_b1!G4</f>
-        <v>27.239000000000001</v>
+        <v>6.4980000000000002</v>
       </c>
       <c r="AA4" s="92">
         <f>[14]LME_PA_l_f0_b1!H4</f>
-        <v>613.19000000000005</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="AB4" s="94">
         <f>[14]LME_PA_l_f0_b1!I4</f>
-        <v>1.12E-107</v>
+        <v>1.1900000000000001E-4</v>
       </c>
       <c r="AC4" s="95">
         <f>[14]LME_PA_l_f0_b1!J4</f>
-        <v>7.8599999999999994E-107</v>
+        <v>9.5E-4</v>
       </c>
       <c r="AD4" s="99">
         <f>[14]LME_PA_l_f0_b1!C5</f>
-        <v>-2.5779999999999998</v>
+        <v>-2.6469999999999998</v>
       </c>
       <c r="AE4" s="92">
         <f>[14]LME_PA_l_f0_b1!D5</f>
-        <v>0.63900000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="AF4" s="93">
         <f>[14]LME_PA_l_f0_b1!E5</f>
-        <v>-3.8290000000000002</v>
+        <v>-4.5279999999999996</v>
       </c>
       <c r="AG4" s="93">
         <f>[14]LME_PA_l_f0_b1!F5</f>
-        <v>-1.3260000000000001</v>
+        <v>-0.76500000000000001</v>
       </c>
       <c r="AH4" s="92">
         <f>[14]LME_PA_l_f0_b1!G5</f>
-        <v>-4.0369999999999999</v>
+        <v>-2.7570000000000001</v>
       </c>
       <c r="AI4" s="92">
         <f>[14]LME_PA_l_f0_b1!H5</f>
-        <v>613.48</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="94">
         <f>[14]LME_PA_l_f0_b1!I5</f>
-        <v>6.0999999999999999E-5</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AK4" s="95">
         <f>[14]LME_PA_l_f0_b1!J5</f>
-        <v>4.2700000000000002E-4</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AL4" s="99">
         <f>[14]LME_PA_l_f0_b1!C6</f>
-        <v>-0.24199999999999999</v>
+        <v>-0.188</v>
       </c>
       <c r="AM4" s="92">
         <f>[14]LME_PA_l_f0_b1!D6</f>
-        <v>0.58799999999999997</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="AN4" s="93">
         <f>[14]LME_PA_l_f0_b1!E6</f>
-        <v>-1.3939999999999999</v>
+        <v>-2.1739999999999999</v>
       </c>
       <c r="AO4" s="93">
         <f>[14]LME_PA_l_f0_b1!F6</f>
-        <v>0.90900000000000003</v>
+        <v>1.798</v>
       </c>
       <c r="AP4" s="92">
         <f>[14]LME_PA_l_f0_b1!G6</f>
-        <v>-0.41199999999999998</v>
+        <v>-0.186</v>
       </c>
       <c r="AQ4" s="92">
         <f>[14]LME_PA_l_f0_b1!H6</f>
-        <v>613.44000000000005</v>
+        <v>0</v>
       </c>
       <c r="AR4" s="94">
         <f>[14]LME_PA_l_f0_b1!I6</f>
-        <v>0.68030000000000002</v>
+        <v>0.99919999999999998</v>
       </c>
       <c r="AS4" s="95">
         <f>[14]LME_PA_l_f0_b1!J6</f>
@@ -16055,43 +16055,43 @@
       </c>
       <c r="AT4" s="99">
         <f>[14]LME_PA_l_f0_b1!C7</f>
-        <v>2.3359999999999999</v>
+        <v>2.4590000000000001</v>
       </c>
       <c r="AU4" s="92">
         <f>[14]LME_PA_l_f0_b1!D7</f>
-        <v>0.27900000000000003</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="AV4" s="93">
         <f>[14]LME_PA_l_f0_b1!E7</f>
-        <v>1.79</v>
+        <v>1.1220000000000001</v>
       </c>
       <c r="AW4" s="93">
         <f>[14]LME_PA_l_f0_b1!F7</f>
-        <v>2.8820000000000001</v>
+        <v>3.7949999999999999</v>
       </c>
       <c r="AX4" s="92">
         <f>[14]LME_PA_l_f0_b1!G7</f>
-        <v>8.3840000000000003</v>
+        <v>3.6040000000000001</v>
       </c>
       <c r="AY4" s="92">
         <f>[14]LME_PA_l_f0_b1!H7</f>
-        <v>613.32000000000005</v>
+        <v>8.08</v>
       </c>
       <c r="AZ4" s="94">
         <f>[14]LME_PA_l_f0_b1!I7</f>
-        <v>3.52E-16</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="BA4" s="95">
         <f>[14]LME_PA_l_f0_b1!J7</f>
-        <v>2.4699999999999999E-15</v>
+        <v>5.4600000000000003E-2</v>
       </c>
       <c r="BB4" s="99">
         <f>[7]LME_PA_l_f0_r2!B3</f>
-        <v>0.58258035813071296</v>
+        <v>0.55641710205239003</v>
       </c>
       <c r="BC4" s="100">
         <f>[7]LME_PA_l_f0_r2!B2</f>
-        <v>0.93416406076052105</v>
+        <v>0.94231449768906905</v>
       </c>
     </row>
     <row r="5" spans="1:55" s="101" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -16100,207 +16100,207 @@
       </c>
       <c r="B5" s="103">
         <f>Intercepts!I10</f>
-        <v>93.153000000000006</v>
+        <v>92.605000000000004</v>
       </c>
       <c r="C5" s="108">
         <f>Intercepts!I11</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="D5" s="108">
         <f>Intercepts!I12</f>
-        <v>98.807000000000002</v>
+        <v>98.281999999999996</v>
       </c>
       <c r="E5" s="141">
         <f>Intercepts!I13</f>
-        <v>98.397999999999996</v>
+        <v>98.17</v>
       </c>
       <c r="F5" s="109">
         <f>[15]LME_PA_h_f0_b1!C2</f>
-        <v>1.367</v>
+        <v>1.145</v>
       </c>
       <c r="G5" s="104">
         <f>[15]LME_PA_h_f0_b1!D2</f>
-        <v>0.82699999999999996</v>
+        <v>1.8109999999999999</v>
       </c>
       <c r="H5" s="105">
         <f>[15]LME_PA_h_f0_b1!E2</f>
-        <v>-0.255</v>
+        <v>-2.4049999999999998</v>
       </c>
       <c r="I5" s="105">
         <f>[15]LME_PA_h_f0_b1!F2</f>
-        <v>2.988</v>
+        <v>4.6950000000000003</v>
       </c>
       <c r="J5" s="104">
         <f>[15]LME_PA_h_f0_b1!G2</f>
-        <v>1.6519999999999999</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="K5" s="104">
         <f>[15]LME_PA_h_f0_b1!H2</f>
-        <v>617.80999999999995</v>
+        <v>0</v>
       </c>
       <c r="L5" s="106">
         <f>[15]LME_PA_h_f0_b1!I2</f>
-        <v>9.9000000000000005E-2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="107">
         <f>[15]LME_PA_h_f0_b1!J2</f>
-        <v>0.69310000000000005</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="N5" s="109">
         <f>[15]LME_PA_h_f0_b1!C3</f>
-        <v>5.6539999999999999</v>
+        <v>5.6769999999999996</v>
       </c>
       <c r="O5" s="104">
         <f>[15]LME_PA_h_f0_b1!D3</f>
-        <v>0.35399999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="P5" s="105">
         <f>[15]LME_PA_h_f0_b1!E3</f>
-        <v>4.96</v>
+        <v>4.452</v>
       </c>
       <c r="Q5" s="105">
         <f>[15]LME_PA_h_f0_b1!F3</f>
-        <v>6.3490000000000002</v>
+        <v>6.9020000000000001</v>
       </c>
       <c r="R5" s="104">
         <f>[15]LME_PA_h_f0_b1!G3</f>
-        <v>15.965</v>
+        <v>9.0860000000000003</v>
       </c>
       <c r="S5" s="104">
         <f>[15]LME_PA_h_f0_b1!H3</f>
-        <v>617.54</v>
+        <v>2.83</v>
       </c>
       <c r="T5" s="106">
         <f>[15]LME_PA_h_f0_b1!I3</f>
-        <v>2.7500000000000002E-48</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="U5" s="107">
         <f>[15]LME_PA_h_f0_b1!I3</f>
-        <v>2.7500000000000002E-48</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="V5" s="109">
         <f>[15]LME_PA_h_f0_b1!C4</f>
-        <v>5.2460000000000004</v>
+        <v>5.5650000000000004</v>
       </c>
       <c r="W5" s="104">
         <f>[15]LME_PA_h_f0_b1!D4</f>
-        <v>0.19700000000000001</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="X5" s="105">
         <f>[15]LME_PA_h_f0_b1!E4</f>
-        <v>4.8600000000000003</v>
+        <v>4.1449999999999996</v>
       </c>
       <c r="Y5" s="105">
         <f>[15]LME_PA_h_f0_b1!F4</f>
-        <v>5.6319999999999997</v>
+        <v>6.9850000000000003</v>
       </c>
       <c r="Z5" s="104">
         <f>[15]LME_PA_h_f0_b1!G4</f>
-        <v>26.620999999999999</v>
+        <v>7.6820000000000004</v>
       </c>
       <c r="AA5" s="104">
         <f>[15]LME_PA_h_f0_b1!H4</f>
-        <v>617.32000000000005</v>
+        <v>9.24</v>
       </c>
       <c r="AB5" s="106">
         <f>[15]LME_PA_h_f0_b1!I4</f>
-        <v>1.43E-104</v>
+        <v>2.6299999999999999E-5</v>
       </c>
       <c r="AC5" s="107">
         <f>[15]LME_PA_h_f0_b1!J4</f>
-        <v>9.9999999999999996E-104</v>
+        <v>2.1100000000000001E-4</v>
       </c>
       <c r="AD5" s="109">
         <f>[15]LME_PA_h_f0_b1!C5</f>
-        <v>4.2880000000000003</v>
+        <v>4.3890000000000002</v>
       </c>
       <c r="AE5" s="104">
         <f>[15]LME_PA_h_f0_b1!D5</f>
-        <v>0.9</v>
+        <v>1.331</v>
       </c>
       <c r="AF5" s="105">
         <f>[15]LME_PA_h_f0_b1!E5</f>
-        <v>2.5230000000000001</v>
+        <v>1.7809999999999999</v>
       </c>
       <c r="AG5" s="105">
         <f>[15]LME_PA_h_f0_b1!F5</f>
-        <v>6.0519999999999996</v>
+        <v>6.9969999999999999</v>
       </c>
       <c r="AH5" s="104">
         <f>[15]LME_PA_h_f0_b1!G5</f>
-        <v>4.7629999999999999</v>
+        <v>3.2989999999999999</v>
       </c>
       <c r="AI5" s="104">
         <f>[15]LME_PA_h_f0_b1!H5</f>
-        <v>617.79999999999995</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="106">
         <f>[15]LME_PA_h_f0_b1!I5</f>
-        <v>2.3800000000000001E-6</v>
+        <v>0.99870000000000003</v>
       </c>
       <c r="AK5" s="107">
         <f>[15]LME_PA_h_f0_b1!J5</f>
-        <v>1.66E-5</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AL5" s="109">
         <f>[15]LME_PA_h_f0_b1!C6</f>
-        <v>3.879</v>
+        <v>4.2770000000000001</v>
       </c>
       <c r="AM5" s="104">
         <f>[15]LME_PA_h_f0_b1!D6</f>
-        <v>0.82899999999999996</v>
+        <v>1.31</v>
       </c>
       <c r="AN5" s="105">
         <f>[15]LME_PA_h_f0_b1!E6</f>
-        <v>2.254</v>
+        <v>1.71</v>
       </c>
       <c r="AO5" s="105">
         <f>[15]LME_PA_h_f0_b1!F6</f>
-        <v>5.5049999999999999</v>
+        <v>6.8449999999999998</v>
       </c>
       <c r="AP5" s="104">
         <f>[15]LME_PA_h_f0_b1!G6</f>
-        <v>4.6769999999999996</v>
+        <v>3.266</v>
       </c>
       <c r="AQ5" s="104">
         <f>[15]LME_PA_h_f0_b1!H6</f>
-        <v>617.75</v>
+        <v>0</v>
       </c>
       <c r="AR5" s="106">
         <f>[15]LME_PA_h_f0_b1!I6</f>
-        <v>3.58E-6</v>
+        <v>0.99880000000000002</v>
       </c>
       <c r="AS5" s="107">
         <f>[15]LME_PA_h_f0_b1!J6</f>
-        <v>2.5000000000000001E-5</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="AT5" s="109">
         <f>[15]LME_PA_h_f0_b1!C7</f>
-        <v>-0.40899999999999997</v>
+        <v>-0.112</v>
       </c>
       <c r="AU5" s="104">
         <f>[15]LME_PA_h_f0_b1!D7</f>
-        <v>0.39100000000000001</v>
+        <v>0.82099999999999995</v>
       </c>
       <c r="AV5" s="105">
         <f>[15]LME_PA_h_f0_b1!E7</f>
-        <v>-1.1739999999999999</v>
+        <v>-1.722</v>
       </c>
       <c r="AW5" s="105">
         <f>[15]LME_PA_h_f0_b1!F7</f>
-        <v>0.35699999999999998</v>
+        <v>1.498</v>
       </c>
       <c r="AX5" s="104">
         <f>[15]LME_PA_h_f0_b1!G7</f>
-        <v>-1.046</v>
+        <v>-0.13600000000000001</v>
       </c>
       <c r="AY5" s="104">
         <f>[15]LME_PA_h_f0_b1!H7</f>
-        <v>617.5</v>
+        <v>6.82</v>
       </c>
       <c r="AZ5" s="106">
         <f>[15]LME_PA_h_f0_b1!I7</f>
-        <v>0.29599999999999999</v>
+        <v>0.89570000000000005</v>
       </c>
       <c r="BA5" s="107">
         <f>[15]LME_PA_h_f0_b1!J7</f>
@@ -16308,15 +16308,15 @@
       </c>
       <c r="BB5" s="109">
         <f>[8]LME_PA_h_f0_r2!B3</f>
-        <v>0.53325993311641395</v>
+        <v>0.46821212674695201</v>
       </c>
       <c r="BC5" s="110">
         <f>[8]LME_PA_h_f0_r2!B2</f>
-        <v>0.89174897721368096</v>
+        <v>0.901950415693481</v>
       </c>
     </row>
     <row r="6" spans="1:55" s="101" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="147" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="103">
@@ -16537,7 +16537,7 @@
       </c>
     </row>
     <row r="7" spans="1:55" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="148" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="83" t="s">
@@ -16757,47 +16757,47 @@
       </c>
       <c r="B8" s="114">
         <f>Intercepts!B3</f>
-        <v>93.504000000000005</v>
+        <v>96.254000000000005</v>
       </c>
       <c r="C8" s="117">
         <f>Intercepts!B4</f>
-        <v>82.188999999999993</v>
+        <v>87.087000000000003</v>
       </c>
       <c r="D8" s="117">
         <f>Intercepts!B5</f>
-        <v>72.698999999999998</v>
+        <v>73.647000000000006</v>
       </c>
       <c r="E8" s="142">
         <f>Intercepts!B5</f>
-        <v>72.698999999999998</v>
+        <v>73.647000000000006</v>
       </c>
       <c r="F8" s="143">
         <f>[16]LME_PA_l_t_b1!C2</f>
-        <v>-11.315</v>
+        <v>-10.675000000000001</v>
       </c>
       <c r="G8" s="144">
         <f>[16]LME_PA_l_t_b1!D2</f>
-        <v>8.2789999999999999</v>
+        <v>18.943999999999999</v>
       </c>
       <c r="H8" s="115">
         <f>[16]LME_PA_l_t_b1!E2</f>
-        <v>-27.542000000000002</v>
+        <v>-47.805999999999997</v>
       </c>
       <c r="I8" s="115">
         <f>[16]LME_PA_l_t_b1!F2</f>
-        <v>4.9119999999999999</v>
+        <v>26.454999999999998</v>
       </c>
       <c r="J8" s="116">
         <f>[16]LME_PA_l_t_b1!G2</f>
-        <v>-1.367</v>
+        <v>-0.56399999999999995</v>
       </c>
       <c r="K8" s="116">
         <f>[16]LME_PA_l_t_b1!H2</f>
-        <v>619.9</v>
+        <v>0.05</v>
       </c>
       <c r="L8" s="97">
         <f>[16]LME_PA_l_t_b1!I2</f>
-        <v>0.17219999999999999</v>
+        <v>0.92359999999999998</v>
       </c>
       <c r="M8" s="98">
         <f>[16]LME_PA_l_t_b1!J2</f>
@@ -16805,95 +16805,95 @@
       </c>
       <c r="N8" s="143">
         <f>[16]LME_PA_l_t_b1!C3</f>
-        <v>-20.805</v>
+        <v>-22.606000000000002</v>
       </c>
       <c r="O8" s="116">
         <f>[16]LME_PA_l_t_b1!D3</f>
-        <v>3.5419999999999998</v>
+        <v>4.3220000000000001</v>
       </c>
       <c r="P8" s="118">
         <f>[16]LME_PA_l_t_b1!E3</f>
-        <v>-27.748000000000001</v>
+        <v>-31.077000000000002</v>
       </c>
       <c r="Q8" s="118">
         <f>[16]LME_PA_l_t_b1!F3</f>
-        <v>-13.862</v>
+        <v>-14.135999999999999</v>
       </c>
       <c r="R8" s="116">
         <f>[16]LME_PA_l_t_b1!G3</f>
-        <v>-5.8730000000000002</v>
+        <v>-5.2309999999999999</v>
       </c>
       <c r="S8" s="116">
         <f>[16]LME_PA_l_t_b1!H3</f>
-        <v>617.97</v>
+        <v>6.16</v>
       </c>
       <c r="T8" s="97">
         <f>[16]LME_PA_l_t_b1!I3</f>
-        <v>6.9900000000000001E-9</v>
+        <v>1.8E-3</v>
       </c>
       <c r="U8" s="98">
         <f>[16]LME_PA_l_t_b1!I3</f>
-        <v>6.9900000000000001E-9</v>
+        <v>1.8E-3</v>
       </c>
       <c r="V8" s="143">
         <f>[16]LME_PA_l_t_b1!C4</f>
-        <v>-23.488</v>
+        <v>-26.52</v>
       </c>
       <c r="W8" s="116">
         <f>[16]LME_PA_l_t_b1!D4</f>
-        <v>1.98</v>
+        <v>7.0949999999999998</v>
       </c>
       <c r="X8" s="118">
         <f>[16]LME_PA_l_t_b1!E4</f>
-        <v>-27.369</v>
+        <v>-40.426000000000002</v>
       </c>
       <c r="Y8" s="118">
         <f>[16]LME_PA_l_t_b1!F4</f>
-        <v>-19.606999999999999</v>
+        <v>-12.614000000000001</v>
       </c>
       <c r="Z8" s="116">
         <f>[16]LME_PA_l_t_b1!G4</f>
-        <v>-11.861000000000001</v>
+        <v>-3.738</v>
       </c>
       <c r="AA8" s="116">
         <f>[16]LME_PA_l_t_b1!H4</f>
-        <v>617.84</v>
+        <v>8.81</v>
       </c>
       <c r="AB8" s="97">
         <f>[16]LME_PA_l_t_b1!I4</f>
-        <v>2.2199999999999999E-29</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AC8" s="98">
         <f>[16]LME_PA_l_t_b1!J4</f>
-        <v>1.55E-28</v>
+        <v>3.8600000000000002E-2</v>
       </c>
       <c r="AD8" s="143">
         <f>[16]LME_PA_l_t_b1!C5</f>
-        <v>-9.49</v>
+        <v>-13.439</v>
       </c>
       <c r="AE8" s="116">
         <f>[16]LME_PA_l_t_b1!D5</f>
-        <v>8.9979999999999993</v>
+        <v>12.378</v>
       </c>
       <c r="AF8" s="118">
         <f>[16]LME_PA_l_t_b1!E5</f>
-        <v>-27.126000000000001</v>
+        <v>-37.701000000000001</v>
       </c>
       <c r="AG8" s="118">
         <f>[16]LME_PA_l_t_b1!F5</f>
-        <v>8.1449999999999996</v>
+        <v>10.821999999999999</v>
       </c>
       <c r="AH8" s="116">
         <f>[16]LME_PA_l_t_b1!G5</f>
-        <v>-1.0549999999999999</v>
+        <v>-1.0860000000000001</v>
       </c>
       <c r="AI8" s="116">
         <f>[16]LME_PA_l_t_b1!H5</f>
-        <v>619.15</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="97">
         <f>[16]LME_PA_l_t_b1!I5</f>
-        <v>0.29199999999999998</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="98">
         <f>[16]LME_PA_l_t_b1!J5</f>
@@ -16901,31 +16901,31 @@
       </c>
       <c r="AL8" s="143">
         <f>[16]LME_PA_l_t_b1!C6</f>
-        <v>-12.173</v>
+        <v>-17.353000000000002</v>
       </c>
       <c r="AM8" s="116">
         <f>[16]LME_PA_l_t_b1!D6</f>
-        <v>8.32</v>
+        <v>12.58</v>
       </c>
       <c r="AN8" s="118">
         <f>[16]LME_PA_l_t_b1!E6</f>
-        <v>-28.48</v>
+        <v>-42.01</v>
       </c>
       <c r="AO8" s="118">
         <f>[16]LME_PA_l_t_b1!F6</f>
-        <v>4.1340000000000003</v>
+        <v>7.3040000000000003</v>
       </c>
       <c r="AP8" s="116">
         <f>[16]LME_PA_l_t_b1!G6</f>
-        <v>-1.4630000000000001</v>
+        <v>-1.379</v>
       </c>
       <c r="AQ8" s="116">
         <f>[16]LME_PA_l_t_b1!H6</f>
-        <v>619.98</v>
+        <v>0</v>
       </c>
       <c r="AR8" s="97">
         <f>[16]LME_PA_l_t_b1!I6</f>
-        <v>0.1439</v>
+        <v>1</v>
       </c>
       <c r="AS8" s="98">
         <f>[16]LME_PA_l_t_b1!J6</f>
@@ -16933,31 +16933,31 @@
       </c>
       <c r="AT8" s="143">
         <f>[16]LME_PA_l_t_b1!C7</f>
-        <v>-2.6829999999999998</v>
+        <v>-3.9129999999999998</v>
       </c>
       <c r="AU8" s="116">
         <f>[16]LME_PA_l_t_b1!D7</f>
-        <v>3.9220000000000002</v>
+        <v>8.3190000000000008</v>
       </c>
       <c r="AV8" s="118">
         <f>[16]LME_PA_l_t_b1!E7</f>
-        <v>-10.37</v>
+        <v>-20.219000000000001</v>
       </c>
       <c r="AW8" s="118">
         <f>[16]LME_PA_l_t_b1!F7</f>
-        <v>5.0039999999999996</v>
+        <v>12.391999999999999</v>
       </c>
       <c r="AX8" s="116">
         <f>[16]LME_PA_l_t_b1!G7</f>
-        <v>-0.68400000000000005</v>
+        <v>-0.47</v>
       </c>
       <c r="AY8" s="116">
         <f>[16]LME_PA_l_t_b1!H7</f>
-        <v>618.83000000000004</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="AZ8" s="97">
         <f>[16]LME_PA_l_t_b1!I7</f>
-        <v>0.49419999999999997</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="BA8" s="98">
         <f>[16]LME_PA_l_t_b1!J7</f>
@@ -16965,32 +16965,32 @@
       </c>
       <c r="BB8" s="119">
         <f>[10]LME_PA_l_t_r2!B3</f>
-        <v>0.593435532261537</v>
+        <v>0.62408082900844397</v>
       </c>
       <c r="BC8" s="120">
         <f>[10]LME_PA_l_t_r2!B2</f>
-        <v>0.73093594252433203</v>
+        <v>0.80115699175044897</v>
       </c>
     </row>
     <row r="9" spans="1:55" s="121" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="165" t="s">
+      <c r="A9" s="149" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="122">
         <f>Intercepts!I10</f>
-        <v>93.153000000000006</v>
+        <v>92.605000000000004</v>
       </c>
       <c r="C9" s="124">
         <f>Intercepts!I11</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
       <c r="D9" s="124">
         <f>Intercepts!I12</f>
-        <v>98.807000000000002</v>
+        <v>98.281999999999996</v>
       </c>
       <c r="E9" s="145">
         <f>Intercepts!I13</f>
-        <v>98.397999999999996</v>
+        <v>98.17</v>
       </c>
       <c r="F9" s="103">
         <f>[17]LME_PA_h_t_b1!C2</f>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="M9" s="107">
         <f>[17]LME_PA_h_t_b1!J2</f>
-        <v>1.19E-9</v>
+        <v>1.3600000000000001E-9</v>
       </c>
       <c r="N9" s="103">
         <f>[17]LME_PA_h_t_b1!C3</f>
@@ -17086,7 +17086,7 @@
       </c>
       <c r="AC9" s="107">
         <f>[17]LME_PA_h_t_b1!J4</f>
-        <v>8.9199999999999998E-9</v>
+        <v>1.02E-8</v>
       </c>
       <c r="AD9" s="103">
         <f>[17]LME_PA_h_t_b1!C5</f>
@@ -17118,7 +17118,7 @@
       </c>
       <c r="AK9" s="107">
         <f>[17]LME_PA_h_t_b1!J5</f>
-        <v>1.2300000000000001E-5</v>
+        <v>1.4E-5</v>
       </c>
       <c r="AL9" s="103">
         <f>[17]LME_PA_h_t_b1!C6</f>
@@ -17150,7 +17150,7 @@
       </c>
       <c r="AS9" s="107">
         <f>[17]LME_PA_h_t_b1!J6</f>
-        <v>5.3800000000000002E-6</v>
+        <v>6.1399999999999997E-6</v>
       </c>
       <c r="AT9" s="103">
         <f>[17]LME_PA_h_t_b1!C7</f>
@@ -17194,7 +17194,7 @@
       </c>
     </row>
     <row r="10" spans="1:55" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="148" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="83" t="s">
@@ -17409,7 +17409,7 @@
       </c>
     </row>
     <row r="11" spans="1:55" s="101" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="150" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="125">
@@ -17631,17 +17631,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="V2:AC2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:BA1"/>
     <mergeCell ref="AD2:AK2"/>
     <mergeCell ref="AT2:BA2"/>
     <mergeCell ref="AL2:AS2"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="N2:U2"/>
-    <mergeCell ref="V2:AC2"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:M6 U4:U6 AC4:AC6 AK4:AK6 AS4:AS6 BA4:BA6 BA8:BA9 AS8:AS9 AK8:AK9 AC8:AC9 U8:U9 M8:M9">
     <cfRule type="cellIs" dxfId="113" priority="102" operator="lessThan">
@@ -18110,7 +18110,7 @@
       </c>
       <c r="B2" s="18">
         <f>Intercepts!B3</f>
-        <v>93.504000000000005</v>
+        <v>96.254000000000005</v>
       </c>
       <c r="C2" s="3">
         <f>Intercepts!B10</f>
@@ -18129,11 +18129,11 @@
       </c>
       <c r="B3" s="18">
         <f>Intercepts!I3</f>
-        <v>87.239000000000004</v>
+        <v>86.994</v>
       </c>
       <c r="C3" s="3">
         <f>Intercepts!I10</f>
-        <v>93.153000000000006</v>
+        <v>92.605000000000004</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>Intercepts!O3</f>
@@ -18183,7 +18183,7 @@
       </c>
       <c r="B6" s="18">
         <f>Intercepts!B4</f>
-        <v>82.188999999999993</v>
+        <v>87.087000000000003</v>
       </c>
       <c r="C6" s="3">
         <f>Intercepts!B11</f>
@@ -18204,11 +18204,11 @@
       </c>
       <c r="B7" s="18">
         <f>Intercepts!I4</f>
-        <v>91.323999999999998</v>
+        <v>91.176000000000002</v>
       </c>
       <c r="C7" s="3">
         <f>Intercepts!I11</f>
-        <v>94.519000000000005</v>
+        <v>93.893000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -18243,7 +18243,7 @@
       </c>
       <c r="B10" s="3">
         <f>Intercepts!B5</f>
-        <v>72.698999999999998</v>
+        <v>73.647000000000006</v>
       </c>
       <c r="C10" s="3">
         <f>Intercepts!B12</f>
@@ -18264,11 +18264,11 @@
       </c>
       <c r="B11" s="3">
         <f>Intercepts!I5</f>
-        <v>88.745999999999995</v>
+        <v>88.528999999999996</v>
       </c>
       <c r="C11" s="3">
         <f>Intercepts!I12</f>
-        <v>98.807000000000002</v>
+        <v>98.281999999999996</v>
       </c>
       <c r="E11" s="32" t="str">
         <f>Intercepts!O11</f>
@@ -18318,7 +18318,7 @@
       </c>
       <c r="B14" s="3">
         <f>Intercepts!B6</f>
-        <v>70.016000000000005</v>
+        <v>69.733999999999995</v>
       </c>
       <c r="C14" s="3">
         <f>Intercepts!B13</f>
@@ -18331,11 +18331,11 @@
       </c>
       <c r="B15" s="3">
         <f>Intercepts!I6</f>
-        <v>91.081999999999994</v>
+        <v>90.988</v>
       </c>
       <c r="C15" s="3">
         <f>Intercepts!I13</f>
-        <v>98.397999999999996</v>
+        <v>98.17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -18368,7 +18368,7 @@
       </c>
       <c r="B19" s="22">
         <f>Intercepts!B3-Intercepts!D3</f>
-        <v>11.165000000000006</v>
+        <v>10.796000000000006</v>
       </c>
       <c r="C19" s="8">
         <f>Intercepts!B10-Intercepts!D10</f>
@@ -18381,11 +18381,11 @@
       </c>
       <c r="B20" s="22">
         <f>Intercepts!I3-Intercepts!K3</f>
-        <v>2.4920000000000044</v>
+        <v>2.3449999999999989</v>
       </c>
       <c r="C20" s="8">
         <f>Intercepts!I10-Intercepts!K10</f>
-        <v>2.6670000000000016</v>
+        <v>2.5400000000000063</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -18411,7 +18411,7 @@
       </c>
       <c r="B23" s="22">
         <f>Intercepts!B4-Intercepts!D4</f>
-        <v>19.824999999999996</v>
+        <v>24.936</v>
       </c>
       <c r="C23" s="8">
         <f>Intercepts!B11-Intercepts!D11</f>
@@ -18424,11 +18424,11 @@
       </c>
       <c r="B24" s="22">
         <f>Intercepts!I4-Intercepts!K4</f>
-        <v>2.7489999999999952</v>
+        <v>2.9230000000000018</v>
       </c>
       <c r="C24" s="8">
         <f>Intercepts!I11-Intercepts!K11</f>
-        <v>3.1290000000000049</v>
+        <v>3.4869999999999948</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -18454,7 +18454,7 @@
       </c>
       <c r="B27" s="8">
         <f>Intercepts!B5-Intercepts!D5</f>
-        <v>12.854999999999997</v>
+        <v>16.801000000000009</v>
       </c>
       <c r="C27" s="8">
         <f>Intercepts!B12-Intercepts!D12</f>
@@ -18467,11 +18467,11 @@
       </c>
       <c r="B28" s="8">
         <f>Intercepts!I5-Intercepts!K5</f>
-        <v>2.5319999999999965</v>
+        <v>2.4909999999999997</v>
       </c>
       <c r="C28" s="8">
         <f>Intercepts!I12-Intercepts!K12</f>
-        <v>2.7409999999999997</v>
+        <v>2.9799999999999898</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -18497,7 +18497,7 @@
       </c>
       <c r="B31" s="8">
         <f>Intercepts!B6-Intercepts!D6</f>
-        <v>11.678000000000004</v>
+        <v>16.794999999999995</v>
       </c>
       <c r="C31" s="8">
         <f>Intercepts!B13-Intercepts!D13</f>
@@ -18510,11 +18510,11 @@
       </c>
       <c r="B32" s="8">
         <f>Intercepts!I6-Intercepts!K6</f>
-        <v>2.5039999999999907</v>
+        <v>2.7789999999999964</v>
       </c>
       <c r="C32" s="8">
         <f>Intercepts!I13-Intercepts!K13</f>
-        <v>2.6880000000000024</v>
+        <v>3.0679999999999978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>